<commit_message>
Actualizacion cedulas resumen y jubilacion
</commit_message>
<xml_diff>
--- a/FASE II - Ejecucion/5000 Activos/5400 Inventarios/5401 - Auditoria de Inventarios.xlsx
+++ b/FASE II - Ejecucion/5000 Activos/5400 Inventarios/5401 - Auditoria de Inventarios.xlsx
@@ -1,34 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos Almeida\Documents\GitHub\VISACOM\FASE II - Ejecucion\5000 Activos\5400 Inventarios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Home\Downloads\VISACOM\FASE II - Ejecucion\5000 Activos\5400 Inventarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E4EFD752-925C-467B-97BA-C835CBD70C05}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20370" windowHeight="2880" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Cedula resumen" sheetId="1" r:id="rId1"/>
+    <sheet name="Cedula Resumen" sheetId="1" r:id="rId1"/>
     <sheet name="Mobiliario" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja2" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -80,9 +68,6 @@
     <t>Con corte al:</t>
   </si>
   <si>
-    <t>Al 31 de Agosto del 2020</t>
-  </si>
-  <si>
     <t>Código</t>
   </si>
   <si>
@@ -104,6 +89,9 @@
     <t>Créditos</t>
   </si>
   <si>
+    <t>Valor</t>
+  </si>
+  <si>
     <t>1.1.3.1</t>
   </si>
   <si>
@@ -323,13 +311,13 @@
     <t>Mobiliario</t>
   </si>
   <si>
-    <t>US$</t>
+    <t>Al 31 de Diciembre del 2020</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="8">
     <numFmt numFmtId="164" formatCode="0.00\ %"/>
     <numFmt numFmtId="165" formatCode="#,##0.00\ ;\(#,##0.00\);\-#\ ;@\ "/>
@@ -913,7 +901,7 @@
     <xf numFmtId="171" fontId="14" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="116">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="170" fontId="16" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
@@ -931,6 +919,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="17" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1019,6 +1008,7 @@
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="17" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -1181,29 +1171,29 @@
     </xf>
   </cellXfs>
   <cellStyles count="23">
-    <cellStyle name="Accent 1 5" xfId="3" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="Accent 2 6" xfId="4" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Accent 3 7" xfId="5" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Accent 4" xfId="6" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="Bad 8" xfId="7" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="cf1" xfId="8" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Currency" xfId="2" builtinId="4"/>
-    <cellStyle name="Error 9" xfId="9" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="Excel Built-in Comma 10" xfId="20" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="Excel Built-in Explanatory Text" xfId="21" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
-    <cellStyle name="Footnote 11" xfId="10" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
-    <cellStyle name="Good 12" xfId="11" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
-    <cellStyle name="Heading (user) 13" xfId="12" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
-    <cellStyle name="Heading 1 14" xfId="13" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
-    <cellStyle name="Heading 2 15" xfId="14" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
-    <cellStyle name="Hyperlink 16" xfId="15" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="Accent 1 5" xfId="3"/>
+    <cellStyle name="Accent 2 6" xfId="4"/>
+    <cellStyle name="Accent 3 7" xfId="5"/>
+    <cellStyle name="Accent 4" xfId="6"/>
+    <cellStyle name="Bad 8" xfId="7"/>
+    <cellStyle name="cf1" xfId="8"/>
+    <cellStyle name="Error 9" xfId="9"/>
+    <cellStyle name="Excel Built-in Comma 10" xfId="20"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="21"/>
+    <cellStyle name="Footnote 11" xfId="10"/>
+    <cellStyle name="Good 12" xfId="11"/>
+    <cellStyle name="Heading (user) 13" xfId="12"/>
+    <cellStyle name="Heading 1 14" xfId="13"/>
+    <cellStyle name="Heading 2 15" xfId="14"/>
+    <cellStyle name="Hyperlink 16" xfId="15"/>
+    <cellStyle name="Millares" xfId="1" builtinId="3"/>
+    <cellStyle name="Moneda" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="22" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
-    <cellStyle name="Note 17" xfId="16" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
-    <cellStyle name="Status 18" xfId="17" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
-    <cellStyle name="Text 19" xfId="18" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
-    <cellStyle name="Warning 20" xfId="19" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
+    <cellStyle name="Normal 2" xfId="22"/>
+    <cellStyle name="Note 17" xfId="16"/>
+    <cellStyle name="Status 18" xfId="17"/>
+    <cellStyle name="Text 19" xfId="18"/>
+    <cellStyle name="Warning 20" xfId="19"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1582,284 +1572,287 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.125" style="66" customWidth="1"/>
-    <col min="2" max="2" width="28.375" style="66" customWidth="1"/>
-    <col min="3" max="3" width="9.5" style="66" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="10.875" style="66" customWidth="1"/>
-    <col min="8" max="8" width="11.125" style="66" customWidth="1"/>
-    <col min="9" max="9" width="30.875" style="66" customWidth="1"/>
-    <col min="10" max="10" width="12.25" style="66" customWidth="1"/>
-    <col min="11" max="11" width="10.25" style="66" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.25" style="67" customWidth="1"/>
-    <col min="13" max="13" width="8.5" style="66" customWidth="1"/>
-    <col min="14" max="16384" width="10.5" style="66"/>
+    <col min="1" max="1" width="11.125" style="68" customWidth="1"/>
+    <col min="2" max="2" width="28.375" style="68" customWidth="1"/>
+    <col min="3" max="3" width="9.5" style="68" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="10.875" style="68" customWidth="1"/>
+    <col min="8" max="8" width="11.125" style="68" customWidth="1"/>
+    <col min="9" max="9" width="30.875" style="68" customWidth="1"/>
+    <col min="10" max="10" width="12.25" style="68" customWidth="1"/>
+    <col min="11" max="11" width="10.25" style="68" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.25" style="69" customWidth="1"/>
+    <col min="13" max="13" width="8.5" style="68" customWidth="1"/>
+    <col min="14" max="16384" width="10.5" style="68"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="106" t="s">
+      <c r="B1" s="108" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="107"/>
-      <c r="D1" s="107"/>
-      <c r="E1" s="107"/>
-      <c r="F1" s="107"/>
-      <c r="G1" s="107"/>
-      <c r="H1" s="108"/>
-      <c r="I1" s="73" t="s">
+      <c r="C1" s="109"/>
+      <c r="D1" s="109"/>
+      <c r="E1" s="109"/>
+      <c r="F1" s="109"/>
+      <c r="G1" s="109"/>
+      <c r="H1" s="110"/>
+      <c r="I1" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="109">
+      <c r="J1" s="111">
         <v>5401</v>
       </c>
-      <c r="K1" s="109"/>
-    </row>
-    <row r="2" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K1" s="111"/>
+    </row>
+    <row r="2" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="106" t="s">
+      <c r="B2" s="108" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="107"/>
-      <c r="D2" s="107"/>
-      <c r="E2" s="107"/>
-      <c r="F2" s="107"/>
-      <c r="G2" s="107"/>
-      <c r="H2" s="108"/>
-      <c r="I2" s="73" t="s">
+      <c r="C2" s="109"/>
+      <c r="D2" s="109"/>
+      <c r="E2" s="109"/>
+      <c r="F2" s="109"/>
+      <c r="G2" s="109"/>
+      <c r="H2" s="110"/>
+      <c r="I2" s="75" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="105" t="s">
+      <c r="J2" s="107" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="105"/>
-    </row>
-    <row r="3" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K2" s="107"/>
+    </row>
+    <row r="3" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="106" t="s">
+      <c r="B3" s="108" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="107"/>
-      <c r="D3" s="107"/>
-      <c r="E3" s="107"/>
-      <c r="F3" s="107"/>
-      <c r="G3" s="107"/>
-      <c r="H3" s="108"/>
-      <c r="I3" s="73" t="s">
+      <c r="C3" s="109"/>
+      <c r="D3" s="109"/>
+      <c r="E3" s="109"/>
+      <c r="F3" s="109"/>
+      <c r="G3" s="109"/>
+      <c r="H3" s="110"/>
+      <c r="I3" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="104">
+      <c r="J3" s="106">
         <v>44134</v>
       </c>
-      <c r="K3" s="104"/>
-    </row>
-    <row r="4" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K3" s="106"/>
+    </row>
+    <row r="4" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="106" t="s">
+      <c r="B4" s="108" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="107"/>
-      <c r="D4" s="107"/>
-      <c r="E4" s="107"/>
-      <c r="F4" s="107"/>
-      <c r="G4" s="107"/>
-      <c r="H4" s="108"/>
-      <c r="I4" s="73" t="s">
+      <c r="C4" s="109"/>
+      <c r="D4" s="109"/>
+      <c r="E4" s="109"/>
+      <c r="F4" s="109"/>
+      <c r="G4" s="109"/>
+      <c r="H4" s="110"/>
+      <c r="I4" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="J4" s="105" t="s">
+      <c r="J4" s="107" t="s">
         <v>13</v>
       </c>
-      <c r="K4" s="105"/>
-    </row>
-    <row r="5" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K4" s="107"/>
+    </row>
+    <row r="5" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="106" t="s">
+      <c r="B5" s="108" t="s">
+        <v>96</v>
+      </c>
+      <c r="C5" s="109"/>
+      <c r="D5" s="109"/>
+      <c r="E5" s="109"/>
+      <c r="F5" s="109"/>
+      <c r="G5" s="109"/>
+      <c r="H5" s="110"/>
+      <c r="I5" s="75" t="s">
+        <v>9</v>
+      </c>
+      <c r="J5" s="112"/>
+      <c r="K5" s="112"/>
+    </row>
+    <row r="6" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L6" s="7"/>
+    </row>
+    <row r="7" spans="1:12" s="6" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="113" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="107"/>
-      <c r="D5" s="107"/>
-      <c r="E5" s="107"/>
-      <c r="F5" s="107"/>
-      <c r="G5" s="107"/>
-      <c r="H5" s="108"/>
-      <c r="I5" s="73" t="s">
-        <v>9</v>
-      </c>
-      <c r="J5" s="110"/>
-      <c r="K5" s="110"/>
-    </row>
-    <row r="7" spans="1:11" s="6" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="111" t="s">
+      <c r="B7" s="114" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="112" t="s">
+      <c r="C7" s="116" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="114" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7" s="7" t="s">
+      <c r="E7" s="115" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="115"/>
+      <c r="G7" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="113" t="s">
-        <v>38</v>
-      </c>
-      <c r="F7" s="113"/>
-      <c r="G7" s="8" t="s">
+      <c r="H7" s="113" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="114" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K7" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="111" t="s">
-        <v>16</v>
-      </c>
-      <c r="I7" s="112" t="s">
-        <v>17</v>
-      </c>
-      <c r="J7" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="K7" s="9" t="s">
+    </row>
+    <row r="8" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="113"/>
+      <c r="B8" s="114"/>
+      <c r="C8" s="117"/>
+      <c r="D8" s="11">
+        <v>44073</v>
+      </c>
+      <c r="E8" s="11" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="111"/>
-      <c r="B8" s="112"/>
-      <c r="C8" s="115"/>
-      <c r="D8" s="10">
-        <v>44073</v>
-      </c>
-      <c r="E8" s="10" t="s">
+      <c r="F8" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="G8" s="12">
+        <v>44196</v>
+      </c>
+      <c r="H8" s="113"/>
+      <c r="I8" s="114"/>
+      <c r="J8" s="11">
+        <v>43830</v>
+      </c>
+      <c r="K8" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="G8" s="11">
-        <v>44196</v>
-      </c>
-      <c r="H8" s="111"/>
-      <c r="I8" s="112"/>
-      <c r="J8" s="10">
-        <v>43830</v>
-      </c>
-      <c r="K8" s="9" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="12"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="20"/>
-      <c r="J9" s="21"/>
-      <c r="K9" s="22"/>
-    </row>
-    <row r="10" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="23"/>
-      <c r="B10" s="24" t="s">
+    </row>
+    <row r="9" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="13"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="23"/>
+    </row>
+    <row r="10" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="24"/>
+      <c r="B10" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="28"/>
-      <c r="I10" s="24" t="s">
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="J10" s="14"/>
+      <c r="J10" s="15"/>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="29" t="s">
+    <row r="11" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="30" t="s">
+      <c r="B11" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="103" t="s">
+      <c r="C11" s="105" t="s">
         <v>95</v>
       </c>
-      <c r="D11" s="14">
+      <c r="D11" s="15">
         <v>47426</v>
       </c>
-      <c r="E11" s="25">
+      <c r="E11" s="26">
         <v>0</v>
       </c>
-      <c r="F11" s="26">
+      <c r="F11" s="27">
         <v>0</v>
       </c>
-      <c r="G11" s="27">
-        <f t="shared" ref="G11:G15" si="0">D11+E11-F11</f>
+      <c r="G11" s="28">
+        <f t="shared" ref="G11:G16" si="0">D11+E11-F11</f>
         <v>47426</v>
       </c>
-      <c r="H11" s="28" t="s">
+      <c r="H11" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="I11" s="31" t="s">
+      <c r="I11" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="J11" s="14">
+      <c r="J11" s="15">
         <v>47426</v>
       </c>
       <c r="K11" s="1">
-        <f t="shared" ref="K11:K15" si="1">G11-J11</f>
+        <f t="shared" ref="K11:K16" si="1">G11-J11</f>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="32" t="s">
+    <row r="12" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14">
+      <c r="C12" s="15"/>
+      <c r="D12" s="15">
         <v>0</v>
       </c>
-      <c r="E12" s="25">
+      <c r="E12" s="26">
         <v>13000</v>
       </c>
-      <c r="F12" s="26">
+      <c r="F12" s="27">
         <v>0</v>
       </c>
-      <c r="G12" s="27">
+      <c r="G12" s="28">
         <f t="shared" si="0"/>
         <v>13000</v>
       </c>
-      <c r="H12" s="33" t="s">
+      <c r="H12" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="I12" s="30" t="s">
+      <c r="I12" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="J12" s="34">
+      <c r="J12" s="35">
         <v>13501</v>
       </c>
       <c r="K12" s="1">
@@ -1867,26 +1860,26 @@
         <v>-501</v>
       </c>
     </row>
-    <row r="13" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="30"/>
-      <c r="B13" s="30"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14">
+    <row r="13" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="31"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15">
         <v>0</v>
       </c>
-      <c r="E13" s="25">
+      <c r="E13" s="26">
         <v>0</v>
       </c>
-      <c r="F13" s="26">
+      <c r="F13" s="27">
         <v>0</v>
       </c>
-      <c r="G13" s="27">
+      <c r="G13" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H13" s="35"/>
-      <c r="I13" s="36"/>
-      <c r="J13" s="34">
+      <c r="H13" s="36"/>
+      <c r="I13" s="37"/>
+      <c r="J13" s="35">
         <v>0</v>
       </c>
       <c r="K13" s="1">
@@ -1894,34 +1887,34 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="30" t="s">
+    <row r="14" spans="1:12" s="38" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="30" t="s">
+      <c r="B14" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14">
+      <c r="C14" s="15"/>
+      <c r="D14" s="15">
         <v>0</v>
       </c>
-      <c r="E14" s="25">
+      <c r="E14" s="26">
         <v>0</v>
       </c>
-      <c r="F14" s="26">
+      <c r="F14" s="27">
         <v>0</v>
       </c>
-      <c r="G14" s="27">
+      <c r="G14" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H14" s="30" t="s">
+      <c r="H14" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="I14" s="30" t="s">
+      <c r="I14" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="J14" s="14">
+      <c r="J14" s="15">
         <v>372</v>
       </c>
       <c r="K14" s="1">
@@ -1929,26 +1922,26 @@
         <v>-372</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="38"/>
+    <row r="15" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="31"/>
       <c r="B15" s="39"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="27">
+      <c r="C15" s="15"/>
+      <c r="D15" s="15">
         <v>0</v>
       </c>
-      <c r="E15" s="25">
+      <c r="E15" s="26">
         <v>0</v>
       </c>
-      <c r="F15" s="26">
+      <c r="F15" s="27">
         <v>0</v>
       </c>
-      <c r="G15" s="40">
+      <c r="G15" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H15" s="41"/>
-      <c r="I15" s="42"/>
-      <c r="J15" s="27">
+      <c r="H15" s="34"/>
+      <c r="I15" s="39"/>
+      <c r="J15" s="35">
         <v>0</v>
       </c>
       <c r="K15" s="1">
@@ -1956,177 +1949,204 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" s="47" customFormat="1" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="43"/>
-      <c r="B16" s="44" t="s">
+    <row r="16" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="40"/>
+      <c r="B16" s="41"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="28">
+        <v>0</v>
+      </c>
+      <c r="E16" s="26">
+        <v>0</v>
+      </c>
+      <c r="F16" s="27">
+        <v>0</v>
+      </c>
+      <c r="G16" s="42">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H16" s="43"/>
+      <c r="I16" s="44"/>
+      <c r="J16" s="28">
+        <v>0</v>
+      </c>
+      <c r="K16" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" s="49" customFormat="1" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="45"/>
+      <c r="B17" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="44"/>
-      <c r="D16" s="45">
-        <f>SUM(D9:D14)</f>
+      <c r="C17" s="46"/>
+      <c r="D17" s="47">
+        <f>SUM(D9:D15)</f>
         <v>47426</v>
       </c>
-      <c r="E16" s="45">
-        <f>SUM(E9:E14)</f>
+      <c r="E17" s="47">
+        <f>SUM(E9:E15)</f>
         <v>13000</v>
       </c>
-      <c r="F16" s="45">
-        <f>SUM(F9:F14)</f>
+      <c r="F17" s="47">
+        <f>SUM(F9:F15)</f>
         <v>0</v>
       </c>
-      <c r="G16" s="46">
-        <f>SUM(G9:G14)</f>
+      <c r="G17" s="48">
+        <f>SUM(G9:G15)</f>
         <v>60426</v>
       </c>
-      <c r="H16" s="43"/>
-      <c r="I16" s="43"/>
-      <c r="J16" s="45">
-        <f>SUM(J9:J14)</f>
+      <c r="H17" s="45"/>
+      <c r="I17" s="45"/>
+      <c r="J17" s="47">
+        <f>SUM(J9:J15)</f>
         <v>61299</v>
       </c>
-      <c r="K16" s="2">
-        <f>SUM(K9:K14)</f>
+      <c r="K17" s="2">
+        <f>SUM(K9:K15)</f>
         <v>-873</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B18" s="48"/>
-      <c r="C18" s="48"/>
-      <c r="D18" s="49" t="s">
+    <row r="18" spans="1:13" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B20" s="50"/>
+      <c r="C20" s="50"/>
+      <c r="D20" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="E18" s="50" t="s">
+      <c r="E20" s="52" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B19" s="3" t="s">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B21" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="51"/>
-      <c r="D19" s="52">
+      <c r="C21" s="53"/>
+      <c r="D21" s="54">
         <v>44073</v>
       </c>
-      <c r="E19" s="52">
+      <c r="E21" s="54">
         <v>43830</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B20" s="53"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="54"/>
-      <c r="E20" s="55"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B21" s="53" t="s">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B22" s="55"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="56"/>
+      <c r="E22" s="57"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B23" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="14"/>
-      <c r="D21" s="56">
+      <c r="C23" s="15"/>
+      <c r="D23" s="58">
         <f>G11</f>
         <v>47426</v>
       </c>
-      <c r="E21" s="57">
+      <c r="E23" s="59">
         <f>J11</f>
         <v>47426</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B22" s="53" t="s">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B24" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="C22" s="14"/>
-      <c r="D22" s="56">
-        <f>SUM(G12:G14)</f>
+      <c r="C24" s="15"/>
+      <c r="D24" s="58">
+        <f>SUM(G12:G15)</f>
         <v>13000</v>
       </c>
-      <c r="E22" s="57">
-        <f>SUM(J12:J14)</f>
+      <c r="E24" s="59">
+        <f>SUM(J12:J15)</f>
         <v>13873</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="53"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="58"/>
-      <c r="E23" s="59"/>
-    </row>
-    <row r="24" spans="1:13" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="51" t="s">
+    <row r="25" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="55"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="60"/>
+      <c r="E25" s="61"/>
+    </row>
+    <row r="26" spans="1:13" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="53" t="s">
         <v>29</v>
       </c>
-      <c r="C24" s="51"/>
-      <c r="D24" s="60">
-        <f>+SUM(D21:D22)</f>
+      <c r="C26" s="53"/>
+      <c r="D26" s="62">
+        <f>+SUM(D23:D24)</f>
         <v>60426</v>
       </c>
-      <c r="E24" s="61">
-        <f>+SUM(E21:E22)</f>
+      <c r="E26" s="63">
+        <f>+SUM(E23:E24)</f>
         <v>61299</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A26" s="62" t="s">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A31" s="64" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="68"/>
-      <c r="C26" s="68"/>
-      <c r="D26" s="68"/>
-      <c r="E26" s="68"/>
-      <c r="F26" s="68"/>
-      <c r="G26" s="68"/>
-      <c r="H26" s="68"/>
-      <c r="I26" s="69"/>
-      <c r="J26" s="70"/>
-      <c r="K26" s="70"/>
-      <c r="L26" s="71"/>
-      <c r="M26" s="70"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A27" s="63" t="s">
+      <c r="B31" s="70"/>
+      <c r="C31" s="70"/>
+      <c r="D31" s="70"/>
+      <c r="E31" s="70"/>
+      <c r="F31" s="70"/>
+      <c r="G31" s="70"/>
+      <c r="H31" s="70"/>
+      <c r="I31" s="71"/>
+      <c r="J31" s="72"/>
+      <c r="K31" s="72"/>
+      <c r="L31" s="73"/>
+      <c r="M31" s="72"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A32" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="I27" s="72"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A28" s="63"/>
-      <c r="I28" s="72"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A29" s="64" t="s">
+      <c r="I32" s="74"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" s="65"/>
+      <c r="I33" s="74"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" s="66" t="s">
         <v>34</v>
       </c>
-      <c r="I29" s="72"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A30" s="63" t="s">
+      <c r="I34" s="74"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="I30" s="72"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A31" s="63" t="s">
-        <v>36</v>
-      </c>
-      <c r="I31" s="72"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A32" s="63"/>
-      <c r="I32" s="72"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33" s="63"/>
-      <c r="I33" s="72"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" s="64" t="s">
-        <v>37</v>
-      </c>
-      <c r="I34" s="72"/>
+      <c r="I35" s="74"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="65" t="s">
+        <v>36</v>
+      </c>
+      <c r="I36" s="74"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37" s="65"/>
+      <c r="I37" s="74"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A38" s="65"/>
+      <c r="I38" s="74"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A39" s="66" t="s">
+        <v>37</v>
+      </c>
+      <c r="I39" s="74"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A41" s="67" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2159,564 +2179,564 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="81" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
     </row>
     <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="79" t="s">
+      <c r="A2" s="81" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="74"/>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
-      <c r="G2" s="74"/>
+      <c r="B2" s="76"/>
+      <c r="C2" s="76"/>
+      <c r="D2" s="76"/>
+      <c r="E2" s="76"/>
+      <c r="F2" s="76"/>
+      <c r="G2" s="76"/>
     </row>
     <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="79" t="s">
+      <c r="A3" s="81" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="74"/>
-      <c r="C3" s="74"/>
-      <c r="D3" s="74"/>
-      <c r="E3" s="74"/>
-      <c r="F3" s="74"/>
-      <c r="G3" s="74"/>
+      <c r="B3" s="76"/>
+      <c r="C3" s="76"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="76"/>
     </row>
     <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="79" t="s">
+      <c r="A4" s="81" t="s">
         <v>45</v>
       </c>
-      <c r="B4" s="74"/>
-      <c r="C4" s="74"/>
-      <c r="D4" s="74"/>
-      <c r="E4" s="74"/>
-      <c r="F4" s="74"/>
-      <c r="G4" s="74"/>
+      <c r="B4" s="76"/>
+      <c r="C4" s="76"/>
+      <c r="D4" s="76"/>
+      <c r="E4" s="76"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="76"/>
     </row>
     <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="87" t="s">
+      <c r="A6" s="89" t="s">
         <v>46</v>
       </c>
-      <c r="B6" s="76" t="s">
+      <c r="B6" s="78" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="75" t="s">
+      <c r="C6" s="77" t="s">
         <v>48</v>
       </c>
-      <c r="D6" s="74"/>
-      <c r="E6" s="86" t="s">
+      <c r="D6" s="76"/>
+      <c r="E6" s="88" t="s">
         <v>49</v>
       </c>
-      <c r="F6" s="74"/>
-      <c r="G6" s="88" t="s">
+      <c r="F6" s="76"/>
+      <c r="G6" s="90" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="81">
+      <c r="A7" s="83">
         <v>43572</v>
       </c>
-      <c r="B7" s="78">
+      <c r="B7" s="80">
         <v>1</v>
       </c>
-      <c r="C7" s="74" t="s">
+      <c r="C7" s="76" t="s">
         <v>51</v>
       </c>
-      <c r="D7" s="74"/>
-      <c r="E7" s="85">
+      <c r="D7" s="76"/>
+      <c r="E7" s="87">
         <v>1344</v>
       </c>
-      <c r="F7" s="74"/>
-      <c r="G7" s="74" t="s">
+      <c r="F7" s="76"/>
+      <c r="G7" s="76" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="81">
+      <c r="A8" s="83">
         <v>43651</v>
       </c>
-      <c r="B8" s="78">
+      <c r="B8" s="80">
         <v>1</v>
       </c>
-      <c r="C8" s="74" t="s">
+      <c r="C8" s="76" t="s">
         <v>53</v>
       </c>
-      <c r="D8" s="74"/>
-      <c r="E8" s="85">
+      <c r="D8" s="76"/>
+      <c r="E8" s="87">
         <v>4700</v>
       </c>
-      <c r="F8" s="74"/>
-      <c r="G8" s="74" t="s">
+      <c r="F8" s="76"/>
+      <c r="G8" s="76" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="81">
+      <c r="A9" s="83">
         <v>43670</v>
       </c>
-      <c r="B9" s="78">
+      <c r="B9" s="80">
         <v>1</v>
       </c>
-      <c r="C9" s="74" t="s">
+      <c r="C9" s="76" t="s">
         <v>54</v>
       </c>
-      <c r="D9" s="74"/>
-      <c r="E9" s="85">
+      <c r="D9" s="76"/>
+      <c r="E9" s="87">
         <v>3905</v>
       </c>
-      <c r="F9" s="74"/>
-      <c r="G9" s="74" t="s">
+      <c r="F9" s="76"/>
+      <c r="G9" s="76" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="81">
+      <c r="A10" s="83">
         <v>43670</v>
       </c>
-      <c r="B10" s="78">
+      <c r="B10" s="80">
         <v>1</v>
       </c>
-      <c r="C10" s="74" t="s">
+      <c r="C10" s="76" t="s">
         <v>55</v>
       </c>
-      <c r="D10" s="74"/>
-      <c r="E10" s="85">
+      <c r="D10" s="76"/>
+      <c r="E10" s="87">
         <v>2055</v>
       </c>
-      <c r="F10" s="74"/>
-      <c r="G10" s="74" t="s">
+      <c r="F10" s="76"/>
+      <c r="G10" s="76" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="81">
+      <c r="A11" s="83">
         <v>43726</v>
       </c>
-      <c r="B11" s="78">
+      <c r="B11" s="80">
         <v>1</v>
       </c>
-      <c r="C11" s="74" t="s">
+      <c r="C11" s="76" t="s">
         <v>56</v>
       </c>
-      <c r="D11" s="74"/>
-      <c r="E11" s="85">
+      <c r="D11" s="76"/>
+      <c r="E11" s="87">
         <v>5524</v>
       </c>
-      <c r="F11" s="74"/>
-      <c r="G11" s="74" t="s">
+      <c r="F11" s="76"/>
+      <c r="G11" s="76" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="81">
+      <c r="A12" s="83">
         <v>43734</v>
       </c>
-      <c r="B12" s="78">
+      <c r="B12" s="80">
         <v>1</v>
       </c>
-      <c r="C12" s="82" t="s">
+      <c r="C12" s="84" t="s">
         <v>58</v>
       </c>
-      <c r="D12" s="74"/>
-      <c r="E12" s="85">
+      <c r="D12" s="76"/>
+      <c r="E12" s="87">
         <v>1010</v>
       </c>
-      <c r="F12" s="74"/>
-      <c r="G12" s="74" t="s">
+      <c r="F12" s="76"/>
+      <c r="G12" s="76" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="81">
+      <c r="A13" s="83">
         <v>43742</v>
       </c>
-      <c r="B13" s="78">
+      <c r="B13" s="80">
         <v>1</v>
       </c>
-      <c r="C13" s="74" t="s">
+      <c r="C13" s="76" t="s">
         <v>59</v>
       </c>
-      <c r="D13" s="74"/>
-      <c r="E13" s="85">
+      <c r="D13" s="76"/>
+      <c r="E13" s="87">
         <v>660</v>
       </c>
-      <c r="F13" s="74"/>
-      <c r="G13" s="74" t="s">
+      <c r="F13" s="76"/>
+      <c r="G13" s="76" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="81">
+      <c r="A14" s="83">
         <v>43752</v>
       </c>
-      <c r="B14" s="78">
+      <c r="B14" s="80">
         <v>1</v>
       </c>
-      <c r="C14" s="74" t="s">
+      <c r="C14" s="76" t="s">
         <v>60</v>
       </c>
-      <c r="D14" s="74"/>
-      <c r="E14" s="85">
+      <c r="D14" s="76"/>
+      <c r="E14" s="87">
         <v>2441</v>
       </c>
-      <c r="F14" s="74"/>
-      <c r="G14" s="74" t="s">
+      <c r="F14" s="76"/>
+      <c r="G14" s="76" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="81">
+      <c r="A15" s="83">
         <v>43752</v>
       </c>
-      <c r="B15" s="78">
+      <c r="B15" s="80">
         <v>1</v>
       </c>
-      <c r="C15" s="74" t="s">
+      <c r="C15" s="76" t="s">
         <v>61</v>
       </c>
-      <c r="D15" s="74"/>
-      <c r="E15" s="85">
+      <c r="D15" s="76"/>
+      <c r="E15" s="87">
         <v>3069</v>
       </c>
-      <c r="F15" s="74"/>
-      <c r="G15" s="74" t="s">
+      <c r="F15" s="76"/>
+      <c r="G15" s="76" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="81">
+      <c r="A16" s="83">
         <v>43613</v>
       </c>
-      <c r="B16" s="78">
+      <c r="B16" s="80">
         <v>1</v>
       </c>
-      <c r="C16" s="74" t="s">
+      <c r="C16" s="76" t="s">
         <v>62</v>
       </c>
-      <c r="D16" s="74"/>
-      <c r="E16" s="85">
+      <c r="D16" s="76"/>
+      <c r="E16" s="87">
         <v>395</v>
       </c>
-      <c r="F16" s="74"/>
-      <c r="G16" s="74" t="s">
+      <c r="F16" s="76"/>
+      <c r="G16" s="76" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="81">
+      <c r="A17" s="83">
         <v>43613</v>
       </c>
-      <c r="B17" s="78">
+      <c r="B17" s="80">
         <v>1</v>
       </c>
-      <c r="C17" s="74" t="s">
+      <c r="C17" s="76" t="s">
         <v>63</v>
       </c>
-      <c r="D17" s="74"/>
-      <c r="E17" s="85">
+      <c r="D17" s="76"/>
+      <c r="E17" s="87">
         <v>550</v>
       </c>
-      <c r="F17" s="74"/>
-      <c r="G17" s="74" t="s">
+      <c r="F17" s="76"/>
+      <c r="G17" s="76" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="81">
+      <c r="A18" s="83">
         <v>43804</v>
       </c>
-      <c r="B18" s="78">
+      <c r="B18" s="80">
         <v>1</v>
       </c>
-      <c r="C18" s="74" t="s">
+      <c r="C18" s="76" t="s">
         <v>64</v>
       </c>
-      <c r="D18" s="74"/>
-      <c r="E18" s="85">
+      <c r="D18" s="76"/>
+      <c r="E18" s="87">
         <v>580</v>
       </c>
-      <c r="F18" s="74"/>
-      <c r="G18" s="74" t="s">
+      <c r="F18" s="76"/>
+      <c r="G18" s="76" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="81">
+      <c r="A19" s="83">
         <v>43573</v>
       </c>
-      <c r="B19" s="78">
+      <c r="B19" s="80">
         <v>1</v>
       </c>
-      <c r="C19" s="74" t="s">
+      <c r="C19" s="76" t="s">
         <v>65</v>
       </c>
-      <c r="D19" s="74"/>
-      <c r="E19" s="85">
+      <c r="D19" s="76"/>
+      <c r="E19" s="87">
         <v>3305</v>
       </c>
-      <c r="F19" s="74"/>
-      <c r="G19" s="74" t="s">
+      <c r="F19" s="76"/>
+      <c r="G19" s="76" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="81">
+      <c r="A20" s="83">
         <v>43657</v>
       </c>
-      <c r="B20" s="78">
+      <c r="B20" s="80">
         <v>2</v>
       </c>
-      <c r="C20" s="74" t="s">
+      <c r="C20" s="76" t="s">
         <v>66</v>
       </c>
-      <c r="D20" s="74"/>
-      <c r="E20" s="85">
+      <c r="D20" s="76"/>
+      <c r="E20" s="87">
         <v>1232</v>
       </c>
-      <c r="F20" s="74"/>
-      <c r="G20" s="74" t="s">
+      <c r="F20" s="76"/>
+      <c r="G20" s="76" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="81">
+      <c r="A21" s="83">
         <v>43784</v>
       </c>
-      <c r="B21" s="78">
+      <c r="B21" s="80">
         <v>1</v>
       </c>
-      <c r="C21" s="74" t="s">
+      <c r="C21" s="76" t="s">
         <v>67</v>
       </c>
-      <c r="D21" s="74"/>
-      <c r="E21" s="85">
+      <c r="D21" s="76"/>
+      <c r="E21" s="87">
         <v>4720</v>
       </c>
-      <c r="F21" s="74"/>
-      <c r="G21" s="74" t="s">
+      <c r="F21" s="76"/>
+      <c r="G21" s="76" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="81">
+      <c r="A22" s="83">
         <v>43789</v>
       </c>
-      <c r="B22" s="78">
+      <c r="B22" s="80">
         <v>2</v>
       </c>
-      <c r="C22" s="74" t="s">
+      <c r="C22" s="76" t="s">
         <v>68</v>
       </c>
-      <c r="D22" s="74"/>
-      <c r="E22" s="85">
+      <c r="D22" s="76"/>
+      <c r="E22" s="87">
         <v>350</v>
       </c>
-      <c r="F22" s="74"/>
-      <c r="G22" s="74" t="s">
+      <c r="F22" s="76"/>
+      <c r="G22" s="76" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="81">
+      <c r="A23" s="83">
         <v>43789</v>
       </c>
-      <c r="B23" s="78">
+      <c r="B23" s="80">
         <v>18</v>
       </c>
-      <c r="C23" s="74" t="s">
+      <c r="C23" s="76" t="s">
         <v>69</v>
       </c>
-      <c r="D23" s="74"/>
-      <c r="E23" s="85">
+      <c r="D23" s="76"/>
+      <c r="E23" s="87">
         <v>7640</v>
       </c>
-      <c r="F23" s="74"/>
-      <c r="G23" s="74" t="s">
+      <c r="F23" s="76"/>
+      <c r="G23" s="76" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="81">
+      <c r="A24" s="83">
         <v>43791</v>
       </c>
-      <c r="B24" s="78">
+      <c r="B24" s="80">
         <v>12</v>
       </c>
-      <c r="C24" s="74" t="s">
+      <c r="C24" s="76" t="s">
         <v>70</v>
       </c>
-      <c r="D24" s="74"/>
-      <c r="E24" s="85">
+      <c r="D24" s="76"/>
+      <c r="E24" s="87">
         <v>846.48</v>
       </c>
-      <c r="F24" s="74"/>
-      <c r="G24" s="74" t="s">
+      <c r="F24" s="76"/>
+      <c r="G24" s="76" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="81">
+      <c r="A25" s="83">
         <v>43795</v>
       </c>
-      <c r="B25" s="78">
+      <c r="B25" s="80">
         <v>4</v>
       </c>
-      <c r="C25" s="74" t="s">
+      <c r="C25" s="76" t="s">
         <v>72</v>
       </c>
-      <c r="D25" s="74"/>
-      <c r="E25" s="85">
+      <c r="D25" s="76"/>
+      <c r="E25" s="87">
         <v>940</v>
       </c>
-      <c r="F25" s="74"/>
-      <c r="G25" s="74" t="s">
+      <c r="F25" s="76"/>
+      <c r="G25" s="76" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="81">
+      <c r="A26" s="83">
         <v>43804</v>
       </c>
-      <c r="B26" s="78">
+      <c r="B26" s="80">
         <v>2</v>
       </c>
-      <c r="C26" s="74" t="s">
+      <c r="C26" s="76" t="s">
         <v>73</v>
       </c>
-      <c r="D26" s="74"/>
-      <c r="E26" s="85">
+      <c r="D26" s="76"/>
+      <c r="E26" s="87">
         <v>790</v>
       </c>
-      <c r="F26" s="74"/>
-      <c r="G26" s="74" t="s">
+      <c r="F26" s="76"/>
+      <c r="G26" s="76" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27" s="81">
+      <c r="A27" s="83">
         <v>43804</v>
       </c>
-      <c r="B27" s="78">
+      <c r="B27" s="80">
         <v>2</v>
       </c>
-      <c r="C27" s="74" t="s">
+      <c r="C27" s="76" t="s">
         <v>75</v>
       </c>
-      <c r="D27" s="74"/>
-      <c r="E27" s="85">
+      <c r="D27" s="76"/>
+      <c r="E27" s="87">
         <v>210</v>
       </c>
-      <c r="F27" s="74"/>
-      <c r="G27" s="74" t="s">
+      <c r="F27" s="76"/>
+      <c r="G27" s="76" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="81">
+      <c r="A28" s="83">
         <v>43804</v>
       </c>
-      <c r="B28" s="78">
+      <c r="B28" s="80">
         <v>4</v>
       </c>
-      <c r="C28" s="74" t="s">
+      <c r="C28" s="76" t="s">
         <v>76</v>
       </c>
-      <c r="D28" s="74"/>
-      <c r="E28" s="85">
+      <c r="D28" s="76"/>
+      <c r="E28" s="87">
         <v>1160</v>
       </c>
-      <c r="F28" s="74"/>
-      <c r="G28" s="74" t="s">
+      <c r="F28" s="76"/>
+      <c r="G28" s="76" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="80"/>
-      <c r="B29" s="74"/>
-      <c r="C29" s="74"/>
-      <c r="D29" s="74"/>
-      <c r="E29" s="83">
+      <c r="A29" s="82"/>
+      <c r="B29" s="76"/>
+      <c r="C29" s="76"/>
+      <c r="D29" s="76"/>
+      <c r="E29" s="85">
         <v>47426.48</v>
       </c>
-      <c r="F29" s="74" t="s">
+      <c r="F29" s="76" t="s">
         <v>77</v>
       </c>
-      <c r="G29" s="77" t="s">
+      <c r="G29" s="79" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="80"/>
-      <c r="B30" s="74"/>
-      <c r="C30" s="74"/>
-      <c r="D30" s="74"/>
-      <c r="E30" s="84"/>
-      <c r="F30" s="74"/>
-      <c r="G30" s="74"/>
+      <c r="A30" s="82"/>
+      <c r="B30" s="76"/>
+      <c r="C30" s="76"/>
+      <c r="D30" s="76"/>
+      <c r="E30" s="86"/>
+      <c r="F30" s="76"/>
+      <c r="G30" s="76"/>
     </row>
     <row r="31" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A31" s="80"/>
-      <c r="B31" s="74"/>
-      <c r="C31" s="74"/>
-      <c r="D31" s="74"/>
-      <c r="E31" s="74"/>
-      <c r="F31" s="74"/>
-      <c r="G31" s="74"/>
+      <c r="A31" s="82"/>
+      <c r="B31" s="76"/>
+      <c r="C31" s="76"/>
+      <c r="D31" s="76"/>
+      <c r="E31" s="76"/>
+      <c r="F31" s="76"/>
+      <c r="G31" s="76"/>
     </row>
     <row r="32" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A32" s="80"/>
-      <c r="B32" s="74"/>
-      <c r="C32" s="74"/>
-      <c r="D32" s="74"/>
-      <c r="E32" s="74"/>
-      <c r="F32" s="74"/>
-      <c r="G32" s="74"/>
+      <c r="A32" s="82"/>
+      <c r="B32" s="76"/>
+      <c r="C32" s="76"/>
+      <c r="D32" s="76"/>
+      <c r="E32" s="76"/>
+      <c r="F32" s="76"/>
+      <c r="G32" s="76"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" s="80"/>
+      <c r="A33" s="82"/>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" s="80"/>
+      <c r="A34" s="82"/>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" s="80"/>
+      <c r="A35" s="82"/>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" s="80"/>
+      <c r="A36" s="82"/>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" s="80"/>
+      <c r="A37" s="82"/>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" s="80"/>
+      <c r="A38" s="82"/>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" s="80"/>
+      <c r="A39" s="82"/>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" s="80"/>
+      <c r="A40" s="82"/>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41" s="80"/>
+      <c r="A41" s="82"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2724,570 +2744,570 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="17.375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="97" t="s">
+      <c r="A1" s="99" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="89"/>
-      <c r="C1" s="89"/>
-      <c r="D1" s="89"/>
-      <c r="E1" s="89"/>
-      <c r="F1" s="89"/>
-      <c r="G1" s="89"/>
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="91"/>
+      <c r="G1" s="91"/>
     </row>
     <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="97" t="s">
+      <c r="A2" s="99" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
+      <c r="B2" s="91"/>
+      <c r="C2" s="91"/>
+      <c r="D2" s="91"/>
+      <c r="E2" s="91"/>
+      <c r="F2" s="91"/>
+      <c r="G2" s="91"/>
     </row>
     <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="97" t="s">
+      <c r="A3" s="99" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="89"/>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
+      <c r="B3" s="91"/>
+      <c r="C3" s="91"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="91"/>
+      <c r="F3" s="91"/>
+      <c r="G3" s="91"/>
     </row>
     <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="97" t="s">
+      <c r="A4" s="99" t="s">
         <v>45</v>
       </c>
-      <c r="B4" s="89"/>
-      <c r="C4" s="89"/>
-      <c r="D4" s="89"/>
-      <c r="E4" s="89"/>
-      <c r="F4" s="89"/>
-      <c r="G4" s="89"/>
+      <c r="B4" s="91"/>
+      <c r="C4" s="91"/>
+      <c r="D4" s="91"/>
+      <c r="E4" s="91"/>
+      <c r="F4" s="91"/>
+      <c r="G4" s="91"/>
     </row>
     <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="99" t="s">
+      <c r="A6" s="101" t="s">
         <v>46</v>
       </c>
-      <c r="B6" s="99" t="s">
+      <c r="B6" s="101" t="s">
         <v>78</v>
       </c>
-      <c r="C6" s="99" t="s">
+      <c r="C6" s="101" t="s">
         <v>79</v>
       </c>
-      <c r="D6" s="99" t="s">
+      <c r="D6" s="101" t="s">
         <v>80</v>
       </c>
-      <c r="E6" s="99" t="s">
+      <c r="E6" s="101" t="s">
         <v>81</v>
       </c>
-      <c r="F6" s="90"/>
-      <c r="G6" s="90"/>
+      <c r="F6" s="92"/>
+      <c r="G6" s="92"/>
     </row>
     <row r="7" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A7" s="91">
+      <c r="A7" s="93">
         <v>43938</v>
       </c>
-      <c r="B7" s="98">
+      <c r="B7" s="100">
         <v>849</v>
       </c>
-      <c r="C7" s="96" t="s">
+      <c r="C7" s="98" t="s">
         <v>82</v>
       </c>
-      <c r="D7" s="100" t="s">
+      <c r="D7" s="102" t="s">
         <v>83</v>
       </c>
-      <c r="E7" s="101">
+      <c r="E7" s="103">
         <v>1344</v>
       </c>
-      <c r="F7" s="92"/>
-      <c r="G7" s="89"/>
+      <c r="F7" s="94"/>
+      <c r="G7" s="91"/>
     </row>
     <row r="8" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="91">
+      <c r="A8" s="93">
         <v>43939</v>
       </c>
-      <c r="B8" s="98">
+      <c r="B8" s="100">
         <v>854</v>
       </c>
-      <c r="C8" s="96" t="s">
+      <c r="C8" s="98" t="s">
         <v>82</v>
       </c>
-      <c r="D8" s="100" t="s">
+      <c r="D8" s="102" t="s">
         <v>83</v>
       </c>
-      <c r="E8" s="101">
+      <c r="E8" s="103">
         <v>3305</v>
       </c>
-      <c r="F8" s="92"/>
-      <c r="G8" s="89"/>
+      <c r="F8" s="94"/>
+      <c r="G8" s="91"/>
     </row>
     <row r="9" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="91">
+      <c r="A9" s="93">
         <v>43979</v>
       </c>
-      <c r="B9" s="98">
+      <c r="B9" s="100">
         <v>870</v>
       </c>
-      <c r="C9" s="96" t="s">
+      <c r="C9" s="98" t="s">
         <v>82</v>
       </c>
-      <c r="D9" s="100" t="s">
+      <c r="D9" s="102" t="s">
         <v>83</v>
       </c>
-      <c r="E9" s="101">
+      <c r="E9" s="103">
         <v>945</v>
       </c>
-      <c r="F9" s="92"/>
-      <c r="G9" s="89"/>
+      <c r="F9" s="94"/>
+      <c r="G9" s="91"/>
     </row>
     <row r="10" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A10" s="91">
+      <c r="A10" s="93">
         <v>44100</v>
       </c>
-      <c r="B10" s="98">
+      <c r="B10" s="100">
         <v>969</v>
       </c>
-      <c r="C10" s="96" t="s">
+      <c r="C10" s="98" t="s">
         <v>82</v>
       </c>
-      <c r="D10" s="100" t="s">
+      <c r="D10" s="102" t="s">
         <v>83</v>
       </c>
-      <c r="E10" s="101">
+      <c r="E10" s="103">
         <v>1010</v>
       </c>
-      <c r="F10" s="92"/>
-      <c r="G10" s="89"/>
+      <c r="F10" s="94"/>
+      <c r="G10" s="91"/>
     </row>
     <row r="11" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A11" s="91">
+      <c r="A11" s="93">
         <v>44036</v>
       </c>
-      <c r="B11" s="98">
+      <c r="B11" s="100">
         <v>929</v>
       </c>
-      <c r="C11" s="96" t="s">
+      <c r="C11" s="98" t="s">
         <v>82</v>
       </c>
-      <c r="D11" s="100" t="s">
+      <c r="D11" s="102" t="s">
         <v>83</v>
       </c>
-      <c r="E11" s="101">
+      <c r="E11" s="103">
         <v>3905</v>
       </c>
-      <c r="F11" s="92"/>
-      <c r="G11" s="89"/>
+      <c r="F11" s="94"/>
+      <c r="G11" s="91"/>
     </row>
     <row r="12" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A12" s="91">
+      <c r="A12" s="93">
         <v>44036</v>
       </c>
-      <c r="B12" s="98">
+      <c r="B12" s="100">
         <v>926</v>
       </c>
-      <c r="C12" s="96" t="s">
+      <c r="C12" s="98" t="s">
         <v>82</v>
       </c>
-      <c r="D12" s="100" t="s">
+      <c r="D12" s="102" t="s">
         <v>83</v>
       </c>
-      <c r="E12" s="101">
+      <c r="E12" s="103">
         <v>2055</v>
       </c>
-      <c r="F12" s="92"/>
-      <c r="G12" s="89"/>
+      <c r="F12" s="94"/>
+      <c r="G12" s="91"/>
     </row>
     <row r="13" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A13" s="91">
+      <c r="A13" s="93">
         <v>44017</v>
       </c>
-      <c r="B13" s="98">
+      <c r="B13" s="100">
         <v>914</v>
       </c>
-      <c r="C13" s="96" t="s">
+      <c r="C13" s="98" t="s">
         <v>82</v>
       </c>
-      <c r="D13" s="100" t="s">
+      <c r="D13" s="102" t="s">
         <v>83</v>
       </c>
-      <c r="E13" s="101">
+      <c r="E13" s="103">
         <v>4700</v>
       </c>
-      <c r="F13" s="92"/>
-      <c r="G13" s="89"/>
+      <c r="F13" s="94"/>
+      <c r="G13" s="91"/>
     </row>
     <row r="14" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A14" s="91">
+      <c r="A14" s="93">
         <v>44108</v>
       </c>
-      <c r="B14" s="98">
+      <c r="B14" s="100">
         <v>154</v>
       </c>
-      <c r="C14" s="96" t="s">
+      <c r="C14" s="98" t="s">
         <v>84</v>
       </c>
-      <c r="D14" s="100" t="s">
+      <c r="D14" s="102" t="s">
         <v>85</v>
       </c>
-      <c r="E14" s="101">
+      <c r="E14" s="103">
         <v>660</v>
       </c>
-      <c r="F14" s="92"/>
-      <c r="G14" s="89"/>
+      <c r="F14" s="94"/>
+      <c r="G14" s="91"/>
     </row>
     <row r="15" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A15" s="91">
+      <c r="A15" s="93">
         <v>44170</v>
       </c>
-      <c r="B15" s="98">
+      <c r="B15" s="100">
         <v>191</v>
       </c>
-      <c r="C15" s="96" t="s">
+      <c r="C15" s="98" t="s">
         <v>84</v>
       </c>
-      <c r="D15" s="100" t="s">
+      <c r="D15" s="102" t="s">
         <v>85</v>
       </c>
-      <c r="E15" s="101">
+      <c r="E15" s="103">
         <v>2740</v>
       </c>
-      <c r="F15" s="92"/>
-      <c r="G15" s="89"/>
+      <c r="F15" s="94"/>
+      <c r="G15" s="91"/>
     </row>
     <row r="16" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A16" s="91">
+      <c r="A16" s="93">
         <v>44118</v>
       </c>
-      <c r="B16" s="98">
+      <c r="B16" s="100">
         <v>550</v>
       </c>
-      <c r="C16" s="96" t="s">
+      <c r="C16" s="98" t="s">
         <v>86</v>
       </c>
-      <c r="D16" s="100" t="s">
+      <c r="D16" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="E16" s="101">
+      <c r="E16" s="103">
         <v>2441</v>
       </c>
-      <c r="F16" s="92"/>
-      <c r="G16" s="89"/>
+      <c r="F16" s="94"/>
+      <c r="G16" s="91"/>
     </row>
     <row r="17" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A17" s="91">
+      <c r="A17" s="93">
         <v>44118</v>
       </c>
-      <c r="B17" s="98">
+      <c r="B17" s="100">
         <v>551</v>
       </c>
-      <c r="C17" s="96" t="s">
+      <c r="C17" s="98" t="s">
         <v>86</v>
       </c>
-      <c r="D17" s="100" t="s">
+      <c r="D17" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="E17" s="101">
+      <c r="E17" s="103">
         <v>3069</v>
       </c>
-      <c r="F17" s="92"/>
-      <c r="G17" s="89"/>
-      <c r="H17" s="89"/>
-      <c r="I17" s="89"/>
+      <c r="F17" s="94"/>
+      <c r="G17" s="91"/>
+      <c r="H17" s="91"/>
+      <c r="I17" s="91"/>
     </row>
     <row r="18" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A18" s="91">
+      <c r="A18" s="93">
         <v>44155</v>
       </c>
-      <c r="B18" s="98">
+      <c r="B18" s="100">
         <v>558</v>
       </c>
-      <c r="C18" s="96" t="s">
+      <c r="C18" s="98" t="s">
         <v>86</v>
       </c>
-      <c r="D18" s="100" t="s">
+      <c r="D18" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="E18" s="101">
+      <c r="E18" s="103">
         <v>7640</v>
       </c>
-      <c r="F18" s="92"/>
-      <c r="G18" s="89"/>
-      <c r="H18" s="89"/>
-      <c r="I18" s="89"/>
+      <c r="F18" s="94"/>
+      <c r="G18" s="91"/>
+      <c r="H18" s="91"/>
+      <c r="I18" s="91"/>
     </row>
     <row r="19" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A19" s="91">
+      <c r="A19" s="93">
         <v>44150</v>
       </c>
-      <c r="B19" s="98">
+      <c r="B19" s="100">
         <v>557</v>
       </c>
-      <c r="C19" s="96" t="s">
+      <c r="C19" s="98" t="s">
         <v>86</v>
       </c>
-      <c r="D19" s="100" t="s">
+      <c r="D19" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="E19" s="101">
+      <c r="E19" s="103">
         <v>4720</v>
       </c>
-      <c r="F19" s="92"/>
-      <c r="G19" s="89"/>
-      <c r="H19" s="89"/>
-      <c r="I19" s="89"/>
+      <c r="F19" s="94"/>
+      <c r="G19" s="91"/>
+      <c r="H19" s="91"/>
+      <c r="I19" s="91"/>
     </row>
     <row r="20" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A20" s="91">
+      <c r="A20" s="93">
         <v>44092</v>
       </c>
-      <c r="B20" s="98">
+      <c r="B20" s="100">
         <v>548</v>
       </c>
-      <c r="C20" s="96" t="s">
+      <c r="C20" s="98" t="s">
         <v>86</v>
       </c>
-      <c r="D20" s="100" t="s">
+      <c r="D20" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="E20" s="101">
+      <c r="E20" s="103">
         <v>5524</v>
       </c>
-      <c r="F20" s="92"/>
-      <c r="G20" s="89"/>
-      <c r="H20" s="89"/>
-      <c r="I20" s="89"/>
+      <c r="F20" s="94"/>
+      <c r="G20" s="91"/>
+      <c r="H20" s="91"/>
+      <c r="I20" s="91"/>
     </row>
     <row r="21" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A21" s="91">
+      <c r="A21" s="93">
         <v>44161</v>
       </c>
-      <c r="B21" s="98">
+      <c r="B21" s="100">
         <v>8274</v>
       </c>
-      <c r="C21" s="96" t="s">
+      <c r="C21" s="98" t="s">
         <v>88</v>
       </c>
-      <c r="D21" s="100" t="s">
+      <c r="D21" s="102" t="s">
         <v>89</v>
       </c>
-      <c r="E21" s="101">
+      <c r="E21" s="103">
         <v>940</v>
       </c>
-      <c r="F21" s="92"/>
-      <c r="G21" s="89"/>
-      <c r="H21" s="89"/>
-      <c r="I21" s="89"/>
+      <c r="F21" s="94"/>
+      <c r="G21" s="91"/>
+      <c r="H21" s="91"/>
+      <c r="I21" s="91"/>
     </row>
     <row r="22" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A22" s="91">
+      <c r="A22" s="93">
         <v>44155</v>
       </c>
-      <c r="B22" s="98">
+      <c r="B22" s="100">
         <v>8267</v>
       </c>
-      <c r="C22" s="96" t="s">
+      <c r="C22" s="98" t="s">
         <v>88</v>
       </c>
-      <c r="D22" s="100" t="s">
+      <c r="D22" s="102" t="s">
         <v>89</v>
       </c>
-      <c r="E22" s="101">
+      <c r="E22" s="103">
         <v>350</v>
       </c>
-      <c r="F22" s="92"/>
-      <c r="G22" s="89"/>
-      <c r="H22" s="89"/>
-      <c r="I22" s="89"/>
+      <c r="F22" s="94"/>
+      <c r="G22" s="91"/>
+      <c r="H22" s="91"/>
+      <c r="I22" s="91"/>
     </row>
     <row r="23" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A23" s="91">
+      <c r="A23" s="93">
         <v>44157</v>
       </c>
-      <c r="B23" s="98">
+      <c r="B23" s="100">
         <v>1504</v>
       </c>
-      <c r="C23" s="96" t="s">
+      <c r="C23" s="98" t="s">
         <v>90</v>
       </c>
-      <c r="D23" s="100" t="s">
+      <c r="D23" s="102" t="s">
         <v>91</v>
       </c>
-      <c r="E23" s="101">
+      <c r="E23" s="103">
         <v>846.48</v>
       </c>
-      <c r="F23" s="92"/>
-      <c r="G23" s="89"/>
-      <c r="H23" s="89"/>
-      <c r="I23" s="89"/>
+      <c r="F23" s="94"/>
+      <c r="G23" s="91"/>
+      <c r="H23" s="91"/>
+      <c r="I23" s="91"/>
     </row>
     <row r="24" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A24" s="94">
+      <c r="A24" s="96">
         <v>44023</v>
       </c>
-      <c r="B24" s="98">
+      <c r="B24" s="100">
         <v>5565</v>
       </c>
-      <c r="C24" s="96" t="s">
+      <c r="C24" s="98" t="s">
         <v>92</v>
       </c>
-      <c r="D24" s="100" t="s">
+      <c r="D24" s="102" t="s">
         <v>93</v>
       </c>
-      <c r="E24" s="101">
+      <c r="E24" s="103">
         <v>1232</v>
       </c>
-      <c r="F24" s="92"/>
-      <c r="G24" s="89"/>
-      <c r="H24" s="89"/>
-      <c r="I24" s="89"/>
+      <c r="F24" s="94"/>
+      <c r="G24" s="91"/>
+      <c r="H24" s="91"/>
+      <c r="I24" s="91"/>
     </row>
     <row r="25" spans="1:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="89"/>
-      <c r="B25" s="89"/>
-      <c r="C25" s="98" t="s">
+      <c r="A25" s="91"/>
+      <c r="B25" s="91"/>
+      <c r="C25" s="100" t="s">
         <v>94</v>
       </c>
-      <c r="D25" s="98"/>
-      <c r="E25" s="102">
+      <c r="D25" s="100"/>
+      <c r="E25" s="104">
         <v>47426.48</v>
       </c>
-      <c r="F25" s="92" t="s">
+      <c r="F25" s="94" t="s">
         <v>77</v>
       </c>
-      <c r="G25" s="92" t="s">
+      <c r="G25" s="94" t="s">
         <v>77</v>
       </c>
-      <c r="H25" s="92" t="s">
+      <c r="H25" s="94" t="s">
         <v>77</v>
       </c>
-      <c r="I25" s="89"/>
+      <c r="I25" s="91"/>
     </row>
     <row r="26" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="89"/>
-      <c r="B26" s="89"/>
-      <c r="C26" s="89"/>
-      <c r="D26" s="89"/>
-      <c r="E26" s="92"/>
-      <c r="F26" s="90"/>
-      <c r="G26" s="90"/>
-      <c r="H26" s="89"/>
-      <c r="I26" s="89"/>
+      <c r="A26" s="91"/>
+      <c r="B26" s="91"/>
+      <c r="C26" s="91"/>
+      <c r="D26" s="91"/>
+      <c r="E26" s="94"/>
+      <c r="F26" s="92"/>
+      <c r="G26" s="92"/>
+      <c r="H26" s="91"/>
+      <c r="I26" s="91"/>
     </row>
     <row r="27" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27" s="89"/>
-      <c r="B27" s="89"/>
-      <c r="C27" s="89"/>
-      <c r="D27" s="89"/>
-      <c r="E27" s="93"/>
-      <c r="F27" s="89"/>
-      <c r="G27" s="89"/>
-      <c r="H27" s="89"/>
-      <c r="I27" s="89"/>
+      <c r="A27" s="91"/>
+      <c r="B27" s="91"/>
+      <c r="C27" s="91"/>
+      <c r="D27" s="91"/>
+      <c r="E27" s="95"/>
+      <c r="F27" s="91"/>
+      <c r="G27" s="91"/>
+      <c r="H27" s="91"/>
+      <c r="I27" s="91"/>
     </row>
     <row r="28" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="89"/>
-      <c r="B28" s="89"/>
-      <c r="C28" s="89"/>
-      <c r="D28" s="89"/>
-      <c r="E28" s="93"/>
-      <c r="F28" s="89"/>
-      <c r="G28" s="89"/>
-      <c r="H28" s="89"/>
-      <c r="I28" s="89"/>
+      <c r="A28" s="91"/>
+      <c r="B28" s="91"/>
+      <c r="C28" s="91"/>
+      <c r="D28" s="91"/>
+      <c r="E28" s="95"/>
+      <c r="F28" s="91"/>
+      <c r="G28" s="91"/>
+      <c r="H28" s="91"/>
+      <c r="I28" s="91"/>
     </row>
     <row r="29" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A29" s="89"/>
-      <c r="B29" s="89"/>
-      <c r="C29" s="89"/>
-      <c r="D29" s="89"/>
-      <c r="E29" s="93"/>
-      <c r="F29" s="89"/>
-      <c r="G29" s="89"/>
-      <c r="H29" s="89"/>
-      <c r="I29" s="89"/>
+      <c r="A29" s="91"/>
+      <c r="B29" s="91"/>
+      <c r="C29" s="91"/>
+      <c r="D29" s="91"/>
+      <c r="E29" s="95"/>
+      <c r="F29" s="91"/>
+      <c r="G29" s="91"/>
+      <c r="H29" s="91"/>
+      <c r="I29" s="91"/>
     </row>
     <row r="30" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A30" s="89"/>
-      <c r="B30" s="89"/>
-      <c r="C30" s="89"/>
-      <c r="D30" s="89"/>
-      <c r="E30" s="93"/>
-      <c r="F30" s="89"/>
-      <c r="G30" s="89"/>
-      <c r="H30" s="89"/>
-      <c r="I30" s="89"/>
+      <c r="A30" s="91"/>
+      <c r="B30" s="91"/>
+      <c r="C30" s="91"/>
+      <c r="D30" s="91"/>
+      <c r="E30" s="95"/>
+      <c r="F30" s="91"/>
+      <c r="G30" s="91"/>
+      <c r="H30" s="91"/>
+      <c r="I30" s="91"/>
     </row>
     <row r="31" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A31" s="89"/>
-      <c r="B31" s="89"/>
-      <c r="C31" s="89"/>
-      <c r="D31" s="89"/>
-      <c r="E31" s="93" t="s">
+      <c r="A31" s="91"/>
+      <c r="B31" s="91"/>
+      <c r="C31" s="91"/>
+      <c r="D31" s="91"/>
+      <c r="E31" s="95" t="s">
         <v>77</v>
       </c>
-      <c r="F31" s="89"/>
-      <c r="G31" s="89"/>
-      <c r="H31" s="89"/>
-      <c r="I31" s="92" t="s">
+      <c r="F31" s="91"/>
+      <c r="G31" s="91"/>
+      <c r="H31" s="91"/>
+      <c r="I31" s="94" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A32" s="89"/>
-      <c r="B32" s="89"/>
-      <c r="C32" s="89"/>
-      <c r="D32" s="89"/>
-      <c r="E32" s="93"/>
-      <c r="F32" s="89"/>
-      <c r="G32" s="89"/>
-      <c r="H32" s="89"/>
-      <c r="I32" s="89"/>
+      <c r="A32" s="91"/>
+      <c r="B32" s="91"/>
+      <c r="C32" s="91"/>
+      <c r="D32" s="91"/>
+      <c r="E32" s="95"/>
+      <c r="F32" s="91"/>
+      <c r="G32" s="91"/>
+      <c r="H32" s="91"/>
+      <c r="I32" s="91"/>
     </row>
     <row r="33" spans="5:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="E33" s="93"/>
+      <c r="E33" s="95"/>
     </row>
     <row r="34" spans="5:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="E34" s="95" t="s">
+      <c r="E34" s="97" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="35" spans="5:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="E35" s="95"/>
+      <c r="E35" s="97"/>
     </row>
     <row r="36" spans="5:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="E36" s="92"/>
+      <c r="E36" s="94"/>
     </row>
     <row r="37" spans="5:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="E37" s="92"/>
+      <c r="E37" s="94"/>
     </row>
     <row r="38" spans="5:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="E38" s="92"/>
+      <c r="E38" s="94"/>
     </row>
     <row r="39" spans="5:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="E39" s="92"/>
+      <c r="E39" s="94"/>
     </row>
     <row r="40" spans="5:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="E40" s="92"/>
+      <c r="E40" s="94"/>
     </row>
     <row r="41" spans="5:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="E41" s="92"/>
+      <c r="E41" s="94"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Informe, costos y gastos
Informe de auditoria, cedulas resumen de costos, gastos, activos y pasivos
</commit_message>
<xml_diff>
--- a/FASE II - Ejecucion/5000 Activos/5400 Inventarios/5401 - Auditoria de Inventarios.xlsx
+++ b/FASE II - Ejecucion/5000 Activos/5400 Inventarios/5401 - Auditoria de Inventarios.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="98">
   <si>
     <t xml:space="preserve">Cliente:</t>
   </si>
@@ -121,6 +121,9 @@
   </si>
   <si>
     <t xml:space="preserve">Mercaderías en Transito</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amortizacion de mobiliario para Eventos ⅓</t>
   </si>
   <si>
     <t xml:space="preserve">Total</t>
@@ -540,7 +543,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -601,8 +604,14 @@
         <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="20">
+  <borders count="27">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -717,10 +726,59 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
       <left style="thin"/>
       <right/>
       <top/>
       <bottom style="double"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right/>
+      <top/>
+      <bottom style="double"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top/>
+      <bottom style="double"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -836,7 +894,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="118">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1029,6 +1087,18 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="170" fontId="18" fillId="11" borderId="6" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="18" fillId="11" borderId="7" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="18" fillId="11" borderId="8" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1101,6 +1171,10 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="170" fontId="18" fillId="10" borderId="15" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="167" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1109,6 +1183,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="170" fontId="18" fillId="10" borderId="16" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="170" fontId="18" fillId="10" borderId="8" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1117,7 +1195,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="18" fillId="0" borderId="15" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="170" fontId="18" fillId="0" borderId="17" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1125,6 +1203,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="170" fontId="5" fillId="0" borderId="14" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1133,15 +1215,47 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="5" fillId="0" borderId="19" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="5" fillId="0" borderId="16" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="10" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="18" fillId="0" borderId="20" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="18" fillId="0" borderId="21" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="5" fillId="0" borderId="22" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1157,7 +1271,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1217,15 +1331,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="174" fontId="17" fillId="0" borderId="19" xfId="33" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="174" fontId="17" fillId="0" borderId="26" xfId="33" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="174" fontId="15" fillId="0" borderId="0" xfId="33" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="174" fontId="17" fillId="0" borderId="0" xfId="33" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1253,15 +1363,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="174" fontId="27" fillId="0" borderId="19" xfId="33" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="33" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="174" fontId="15" fillId="0" borderId="0" xfId="33" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="174" fontId="27" fillId="0" borderId="26" xfId="33" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1360,10 +1462,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M41"/>
+  <dimension ref="A1:M44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F23" activeCellId="0" sqref="F23"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15:G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1375,7 +1477,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="30.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="12.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="10.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="10.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="12.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="8.5"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="14" style="1" width="10.5"/>
@@ -1711,20 +1813,22 @@
     </row>
     <row r="15" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="38"/>
-      <c r="B15" s="47"/>
+      <c r="B15" s="47" t="s">
+        <v>33</v>
+      </c>
       <c r="C15" s="21"/>
-      <c r="D15" s="21" t="n">
+      <c r="D15" s="48" t="n">
         <v>0</v>
       </c>
-      <c r="E15" s="32" t="n">
+      <c r="E15" s="49" t="n">
         <v>0</v>
       </c>
-      <c r="F15" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="G15" s="34" t="n">
+      <c r="F15" s="50" t="n">
+        <v>15808.83</v>
+      </c>
+      <c r="G15" s="48" t="n">
         <f aca="false">D15+E15-F15</f>
-        <v>0</v>
+        <v>-15808.83</v>
       </c>
       <c r="H15" s="42"/>
       <c r="I15" s="47"/>
@@ -1733,12 +1837,12 @@
       </c>
       <c r="K15" s="36" t="n">
         <f aca="false">G15-J15</f>
-        <v>0</v>
+        <v>-15808.83</v>
       </c>
     </row>
     <row r="16" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="48"/>
-      <c r="B16" s="49"/>
+      <c r="A16" s="51"/>
+      <c r="B16" s="52"/>
       <c r="C16" s="21"/>
       <c r="D16" s="34" t="n">
         <v>0</v>
@@ -1749,12 +1853,12 @@
       <c r="F16" s="33" t="n">
         <v>0</v>
       </c>
-      <c r="G16" s="50" t="n">
+      <c r="G16" s="53" t="n">
         <f aca="false">D16+E16-F16</f>
         <v>0</v>
       </c>
-      <c r="H16" s="51"/>
-      <c r="I16" s="52"/>
+      <c r="H16" s="54"/>
+      <c r="I16" s="55"/>
       <c r="J16" s="34" t="n">
         <v>0</v>
       </c>
@@ -1763,178 +1867,210 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" s="58" customFormat="true" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="53"/>
-      <c r="B17" s="54" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" s="54"/>
-      <c r="D17" s="55" t="n">
+    <row r="17" s="61" customFormat="true" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="56"/>
+      <c r="B17" s="57" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="57"/>
+      <c r="D17" s="58" t="n">
         <f aca="false">SUM(D9:D15)</f>
         <v>47426</v>
       </c>
-      <c r="E17" s="55" t="n">
+      <c r="E17" s="58" t="n">
         <f aca="false">SUM(E9:E15)</f>
         <v>13000</v>
       </c>
-      <c r="F17" s="55" t="n">
+      <c r="F17" s="58" t="n">
         <f aca="false">SUM(F9:F15)</f>
-        <v>0</v>
-      </c>
-      <c r="G17" s="56" t="n">
+        <v>15808.83</v>
+      </c>
+      <c r="G17" s="59" t="n">
         <f aca="false">SUM(G9:G15)</f>
-        <v>60426</v>
-      </c>
-      <c r="H17" s="53"/>
-      <c r="I17" s="53"/>
-      <c r="J17" s="55" t="n">
+        <v>44617.17</v>
+      </c>
+      <c r="H17" s="56"/>
+      <c r="I17" s="56"/>
+      <c r="J17" s="58" t="n">
         <f aca="false">SUM(J9:J15)</f>
         <v>61299</v>
       </c>
-      <c r="K17" s="57" t="n">
+      <c r="K17" s="60" t="n">
         <f aca="false">SUM(K9:K15)</f>
-        <v>-873</v>
+        <v>-16681.83</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="59"/>
-      <c r="C20" s="59"/>
-      <c r="D20" s="60" t="s">
-        <v>34</v>
-      </c>
-      <c r="E20" s="61" t="s">
-        <v>34</v>
+      <c r="B20" s="62"/>
+      <c r="C20" s="62"/>
+      <c r="D20" s="63" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20" s="64" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="62" t="s">
-        <v>35</v>
-      </c>
-      <c r="C21" s="63"/>
-      <c r="D21" s="64" t="n">
-        <v>44073</v>
-      </c>
-      <c r="E21" s="64" t="n">
+      <c r="B21" s="65" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="66"/>
+      <c r="D21" s="67" t="n">
+        <v>44196</v>
+      </c>
+      <c r="E21" s="67" t="n">
         <v>43830</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="65"/>
-      <c r="C22" s="21"/>
-      <c r="D22" s="66"/>
-      <c r="E22" s="67"/>
-    </row>
-    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="65" t="s">
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="68"/>
+      <c r="C22" s="69"/>
+      <c r="D22" s="70"/>
+      <c r="E22" s="71"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="68" t="s">
         <v>27</v>
       </c>
-      <c r="C23" s="21"/>
-      <c r="D23" s="68" t="n">
+      <c r="C23" s="72"/>
+      <c r="D23" s="73" t="n">
         <f aca="false">G11</f>
         <v>47426</v>
       </c>
-      <c r="E23" s="69" t="n">
+      <c r="E23" s="74" t="n">
         <f aca="false">J11</f>
         <v>47426</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="65" t="s">
-        <v>36</v>
-      </c>
-      <c r="C24" s="21"/>
-      <c r="D24" s="68" t="n">
-        <f aca="false">SUM(G12:G15)</f>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="68" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" s="72"/>
+      <c r="D24" s="73" t="n">
+        <f aca="false">SUM(G12:G14)</f>
         <v>13000</v>
       </c>
-      <c r="E24" s="69" t="n">
+      <c r="E24" s="74" t="n">
         <f aca="false">SUM(J12:J15)</f>
         <v>13873</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="65"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="70"/>
-      <c r="E25" s="71"/>
-    </row>
-    <row r="26" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="63" t="s">
-        <v>33</v>
-      </c>
-      <c r="C26" s="63"/>
-      <c r="D26" s="72" t="n">
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="68"/>
+      <c r="C25" s="72"/>
+      <c r="D25" s="75"/>
+      <c r="E25" s="76"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="66" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" s="77"/>
+      <c r="D26" s="78" t="n">
         <f aca="false">+SUM(D23:D24)</f>
         <v>60426</v>
       </c>
-      <c r="E26" s="73" t="n">
+      <c r="E26" s="79" t="n">
         <f aca="false">+SUM(E23:E24)</f>
         <v>61299</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="74" t="s">
-        <v>37</v>
-      </c>
-      <c r="B31" s="75"/>
-      <c r="C31" s="75"/>
-      <c r="D31" s="75"/>
-      <c r="E31" s="75"/>
-      <c r="F31" s="75"/>
-      <c r="G31" s="75"/>
-      <c r="H31" s="75"/>
-      <c r="I31" s="76"/>
-      <c r="J31" s="77"/>
-      <c r="K31" s="77"/>
-      <c r="L31" s="78"/>
-      <c r="M31" s="77"/>
-    </row>
-    <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="79" t="s">
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="80"/>
+      <c r="C27" s="80"/>
+      <c r="D27" s="81"/>
+      <c r="E27" s="82"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="83" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28" s="84"/>
+      <c r="D28" s="85" t="n">
+        <f aca="false">G15</f>
+        <v>-15808.83</v>
+      </c>
+      <c r="E28" s="86" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="77"/>
+      <c r="C29" s="77"/>
+      <c r="D29" s="87" t="n">
+        <f aca="false">D26+D28</f>
+        <v>44617.17</v>
+      </c>
+      <c r="E29" s="87" t="n">
+        <f aca="false">E26+E28</f>
+        <v>61299</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="88" t="s">
         <v>38</v>
       </c>
-      <c r="I32" s="80"/>
-    </row>
-    <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="79"/>
-      <c r="I33" s="80"/>
-    </row>
-    <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="81" t="s">
+      <c r="B34" s="89"/>
+      <c r="C34" s="89"/>
+      <c r="D34" s="89"/>
+      <c r="E34" s="89"/>
+      <c r="F34" s="89"/>
+      <c r="G34" s="89"/>
+      <c r="H34" s="89"/>
+      <c r="I34" s="90"/>
+      <c r="J34" s="91"/>
+      <c r="K34" s="91"/>
+      <c r="L34" s="92"/>
+      <c r="M34" s="91"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="93" t="s">
         <v>39</v>
       </c>
-      <c r="I34" s="80"/>
-    </row>
-    <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="79" t="s">
+      <c r="I35" s="94"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="93"/>
+      <c r="I36" s="94"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="95" t="s">
         <v>40</v>
       </c>
-      <c r="I35" s="80"/>
-    </row>
-    <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="79" t="s">
+      <c r="I37" s="94"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="93" t="s">
         <v>41</v>
       </c>
-      <c r="I36" s="80"/>
-    </row>
-    <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="79"/>
-      <c r="I37" s="80"/>
-    </row>
-    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="79"/>
-      <c r="I38" s="80"/>
+      <c r="I38" s="94"/>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="81" t="s">
+      <c r="A39" s="93" t="s">
         <v>42</v>
       </c>
-      <c r="I39" s="80"/>
+      <c r="I39" s="94"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="93"/>
+      <c r="I40" s="94"/>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="82" t="s">
+      <c r="A41" s="93"/>
+      <c r="I41" s="94"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="95" t="s">
         <v>43</v>
+      </c>
+      <c r="I42" s="94"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="96" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1974,560 +2110,560 @@
   <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L29" activeCellId="0" sqref="L29"/>
+      <selection pane="topLeft" activeCell="L29" activeCellId="1" sqref="D15:G15 L29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.609375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.59375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="83" t="s">
-        <v>44</v>
-      </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
-      <c r="F1" s="84"/>
-      <c r="G1" s="84"/>
+      <c r="A1" s="97" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="98"/>
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="98"/>
+      <c r="G1" s="98"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="83" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
+      <c r="A2" s="97" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="83" t="s">
-        <v>46</v>
-      </c>
-      <c r="B3" s="84"/>
-      <c r="C3" s="84"/>
-      <c r="D3" s="84"/>
-      <c r="E3" s="84"/>
-      <c r="F3" s="84"/>
-      <c r="G3" s="84"/>
+      <c r="A3" s="97" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="98"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="83" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" s="84"/>
-      <c r="C4" s="84"/>
-      <c r="D4" s="84"/>
-      <c r="E4" s="84"/>
-      <c r="F4" s="84"/>
-      <c r="G4" s="84"/>
+      <c r="A4" s="97" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="98"/>
+      <c r="C4" s="98"/>
+      <c r="D4" s="98"/>
+      <c r="E4" s="98"/>
+      <c r="F4" s="98"/>
+      <c r="G4" s="98"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="85" t="s">
-        <v>48</v>
-      </c>
-      <c r="B6" s="86" t="s">
+      <c r="A6" s="99" t="s">
         <v>49</v>
       </c>
-      <c r="C6" s="87" t="s">
+      <c r="B6" s="100" t="s">
         <v>50</v>
       </c>
-      <c r="D6" s="84"/>
-      <c r="E6" s="88" t="s">
+      <c r="C6" s="101" t="s">
         <v>51</v>
       </c>
-      <c r="F6" s="84"/>
-      <c r="G6" s="89" t="s">
+      <c r="D6" s="98"/>
+      <c r="E6" s="102" t="s">
         <v>52</v>
       </c>
+      <c r="F6" s="98"/>
+      <c r="G6" s="103" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="90" t="n">
+      <c r="A7" s="104" t="n">
         <v>43572</v>
       </c>
-      <c r="B7" s="91" t="n">
+      <c r="B7" s="105" t="n">
         <v>1</v>
       </c>
-      <c r="C7" s="84" t="s">
-        <v>53</v>
-      </c>
-      <c r="D7" s="84"/>
-      <c r="E7" s="92" t="n">
+      <c r="C7" s="98" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="98"/>
+      <c r="E7" s="106" t="n">
         <v>1344</v>
       </c>
-      <c r="F7" s="84"/>
-      <c r="G7" s="84" t="s">
-        <v>54</v>
+      <c r="F7" s="98"/>
+      <c r="G7" s="98" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="90" t="n">
+      <c r="A8" s="104" t="n">
         <v>43651</v>
       </c>
-      <c r="B8" s="91" t="n">
+      <c r="B8" s="105" t="n">
         <v>1</v>
       </c>
-      <c r="C8" s="84" t="s">
+      <c r="C8" s="98" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="98"/>
+      <c r="E8" s="106" t="n">
+        <v>4700</v>
+      </c>
+      <c r="F8" s="98"/>
+      <c r="G8" s="98" t="s">
         <v>55</v>
       </c>
-      <c r="D8" s="84"/>
-      <c r="E8" s="92" t="n">
-        <v>4700</v>
-      </c>
-      <c r="F8" s="84"/>
-      <c r="G8" s="84" t="s">
-        <v>54</v>
-      </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="90" t="n">
+      <c r="A9" s="104" t="n">
         <v>43670</v>
       </c>
-      <c r="B9" s="91" t="n">
+      <c r="B9" s="105" t="n">
         <v>1</v>
       </c>
-      <c r="C9" s="84" t="s">
-        <v>56</v>
-      </c>
-      <c r="D9" s="84"/>
-      <c r="E9" s="92" t="n">
+      <c r="C9" s="98" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="98"/>
+      <c r="E9" s="106" t="n">
         <v>3905</v>
       </c>
-      <c r="F9" s="84"/>
-      <c r="G9" s="84" t="s">
-        <v>54</v>
+      <c r="F9" s="98"/>
+      <c r="G9" s="98" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="90" t="n">
+      <c r="A10" s="104" t="n">
         <v>43670</v>
       </c>
-      <c r="B10" s="91" t="n">
+      <c r="B10" s="105" t="n">
         <v>1</v>
       </c>
-      <c r="C10" s="84" t="s">
-        <v>57</v>
-      </c>
-      <c r="D10" s="84"/>
-      <c r="E10" s="92" t="n">
+      <c r="C10" s="98" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="98"/>
+      <c r="E10" s="106" t="n">
         <v>2055</v>
       </c>
-      <c r="F10" s="84"/>
-      <c r="G10" s="84" t="s">
-        <v>54</v>
+      <c r="F10" s="98"/>
+      <c r="G10" s="98" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="90" t="n">
+      <c r="A11" s="104" t="n">
         <v>43726</v>
       </c>
-      <c r="B11" s="91" t="n">
+      <c r="B11" s="105" t="n">
         <v>1</v>
       </c>
-      <c r="C11" s="84" t="s">
-        <v>58</v>
-      </c>
-      <c r="D11" s="84"/>
-      <c r="E11" s="92" t="n">
+      <c r="C11" s="98" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="98"/>
+      <c r="E11" s="106" t="n">
         <v>5524</v>
       </c>
-      <c r="F11" s="84"/>
-      <c r="G11" s="84" t="s">
-        <v>59</v>
+      <c r="F11" s="98"/>
+      <c r="G11" s="98" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="90" t="n">
+      <c r="A12" s="104" t="n">
         <v>43734</v>
       </c>
-      <c r="B12" s="91" t="n">
+      <c r="B12" s="105" t="n">
         <v>1</v>
       </c>
-      <c r="C12" s="93" t="s">
+      <c r="C12" s="107" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" s="98"/>
+      <c r="E12" s="106" t="n">
+        <v>1010</v>
+      </c>
+      <c r="F12" s="98"/>
+      <c r="G12" s="98" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="104" t="n">
+        <v>43742</v>
+      </c>
+      <c r="B13" s="105" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" s="98" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13" s="98"/>
+      <c r="E13" s="106" t="n">
+        <v>660</v>
+      </c>
+      <c r="F13" s="98"/>
+      <c r="G13" s="98" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="104" t="n">
+        <v>43752</v>
+      </c>
+      <c r="B14" s="105" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" s="98" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" s="98"/>
+      <c r="E14" s="106" t="n">
+        <v>2441</v>
+      </c>
+      <c r="F14" s="98"/>
+      <c r="G14" s="98" t="s">
         <v>60</v>
       </c>
-      <c r="D12" s="84"/>
-      <c r="E12" s="92" t="n">
-        <v>1010</v>
-      </c>
-      <c r="F12" s="84"/>
-      <c r="G12" s="84" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="90" t="n">
-        <v>43742</v>
-      </c>
-      <c r="B13" s="91" t="n">
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="104" t="n">
+        <v>43752</v>
+      </c>
+      <c r="B15" s="105" t="n">
         <v>1</v>
       </c>
-      <c r="C13" s="84" t="s">
-        <v>61</v>
-      </c>
-      <c r="D13" s="84"/>
-      <c r="E13" s="92" t="n">
-        <v>660</v>
-      </c>
-      <c r="F13" s="84"/>
-      <c r="G13" s="84" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="90" t="n">
-        <v>43752</v>
-      </c>
-      <c r="B14" s="91" t="n">
+      <c r="C15" s="98" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" s="98"/>
+      <c r="E15" s="106" t="n">
+        <v>3069</v>
+      </c>
+      <c r="F15" s="98"/>
+      <c r="G15" s="98" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="104" t="n">
+        <v>43613</v>
+      </c>
+      <c r="B16" s="105" t="n">
         <v>1</v>
       </c>
-      <c r="C14" s="84" t="s">
-        <v>62</v>
-      </c>
-      <c r="D14" s="84"/>
-      <c r="E14" s="92" t="n">
-        <v>2441</v>
-      </c>
-      <c r="F14" s="84"/>
-      <c r="G14" s="84" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="90" t="n">
-        <v>43752</v>
-      </c>
-      <c r="B15" s="91" t="n">
+      <c r="C16" s="98" t="s">
+        <v>65</v>
+      </c>
+      <c r="D16" s="98"/>
+      <c r="E16" s="106" t="n">
+        <v>395</v>
+      </c>
+      <c r="F16" s="98"/>
+      <c r="G16" s="98" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="104" t="n">
+        <v>43613</v>
+      </c>
+      <c r="B17" s="105" t="n">
         <v>1</v>
       </c>
-      <c r="C15" s="84" t="s">
-        <v>63</v>
-      </c>
-      <c r="D15" s="84"/>
-      <c r="E15" s="92" t="n">
-        <v>3069</v>
-      </c>
-      <c r="F15" s="84"/>
-      <c r="G15" s="84" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="90" t="n">
-        <v>43613</v>
-      </c>
-      <c r="B16" s="91" t="n">
+      <c r="C17" s="98" t="s">
+        <v>66</v>
+      </c>
+      <c r="D17" s="98"/>
+      <c r="E17" s="106" t="n">
+        <v>550</v>
+      </c>
+      <c r="F17" s="98"/>
+      <c r="G17" s="98" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="104" t="n">
+        <v>43804</v>
+      </c>
+      <c r="B18" s="105" t="n">
         <v>1</v>
       </c>
-      <c r="C16" s="84" t="s">
-        <v>64</v>
-      </c>
-      <c r="D16" s="84"/>
-      <c r="E16" s="92" t="n">
-        <v>395</v>
-      </c>
-      <c r="F16" s="84"/>
-      <c r="G16" s="84" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="90" t="n">
-        <v>43613</v>
-      </c>
-      <c r="B17" s="91" t="n">
+      <c r="C18" s="98" t="s">
+        <v>67</v>
+      </c>
+      <c r="D18" s="98"/>
+      <c r="E18" s="106" t="n">
+        <v>580</v>
+      </c>
+      <c r="F18" s="98"/>
+      <c r="G18" s="98" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="104" t="n">
+        <v>43573</v>
+      </c>
+      <c r="B19" s="105" t="n">
         <v>1</v>
       </c>
-      <c r="C17" s="84" t="s">
-        <v>65</v>
-      </c>
-      <c r="D17" s="84"/>
-      <c r="E17" s="92" t="n">
-        <v>550</v>
-      </c>
-      <c r="F17" s="84"/>
-      <c r="G17" s="84" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="90" t="n">
+      <c r="C19" s="98" t="s">
+        <v>68</v>
+      </c>
+      <c r="D19" s="98"/>
+      <c r="E19" s="106" t="n">
+        <v>3305</v>
+      </c>
+      <c r="F19" s="98"/>
+      <c r="G19" s="98" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="104" t="n">
+        <v>43657</v>
+      </c>
+      <c r="B20" s="105" t="n">
+        <v>2</v>
+      </c>
+      <c r="C20" s="98" t="s">
+        <v>69</v>
+      </c>
+      <c r="D20" s="98"/>
+      <c r="E20" s="106" t="n">
+        <v>1232</v>
+      </c>
+      <c r="F20" s="98"/>
+      <c r="G20" s="98" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="104" t="n">
+        <v>43784</v>
+      </c>
+      <c r="B21" s="105" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" s="98" t="s">
+        <v>70</v>
+      </c>
+      <c r="D21" s="98"/>
+      <c r="E21" s="106" t="n">
+        <v>4720</v>
+      </c>
+      <c r="F21" s="98"/>
+      <c r="G21" s="98" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="104" t="n">
+        <v>43789</v>
+      </c>
+      <c r="B22" s="105" t="n">
+        <v>2</v>
+      </c>
+      <c r="C22" s="98" t="s">
+        <v>71</v>
+      </c>
+      <c r="D22" s="98"/>
+      <c r="E22" s="106" t="n">
+        <v>350</v>
+      </c>
+      <c r="F22" s="98"/>
+      <c r="G22" s="98" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="104" t="n">
+        <v>43789</v>
+      </c>
+      <c r="B23" s="105" t="n">
+        <v>18</v>
+      </c>
+      <c r="C23" s="98" t="s">
+        <v>72</v>
+      </c>
+      <c r="D23" s="98"/>
+      <c r="E23" s="106" t="n">
+        <v>7640</v>
+      </c>
+      <c r="F23" s="98"/>
+      <c r="G23" s="98" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="104" t="n">
+        <v>43791</v>
+      </c>
+      <c r="B24" s="105" t="n">
+        <v>12</v>
+      </c>
+      <c r="C24" s="98" t="s">
+        <v>73</v>
+      </c>
+      <c r="D24" s="98"/>
+      <c r="E24" s="106" t="n">
+        <v>846.48</v>
+      </c>
+      <c r="F24" s="98"/>
+      <c r="G24" s="98" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="104" t="n">
+        <v>43795</v>
+      </c>
+      <c r="B25" s="105" t="n">
+        <v>4</v>
+      </c>
+      <c r="C25" s="98" t="s">
+        <v>75</v>
+      </c>
+      <c r="D25" s="98"/>
+      <c r="E25" s="106" t="n">
+        <v>940</v>
+      </c>
+      <c r="F25" s="98"/>
+      <c r="G25" s="98" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="104" t="n">
         <v>43804</v>
       </c>
-      <c r="B18" s="91" t="n">
-        <v>1</v>
-      </c>
-      <c r="C18" s="84" t="s">
-        <v>66</v>
-      </c>
-      <c r="D18" s="84"/>
-      <c r="E18" s="92" t="n">
-        <v>580</v>
-      </c>
-      <c r="F18" s="84"/>
-      <c r="G18" s="84" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="90" t="n">
-        <v>43573</v>
-      </c>
-      <c r="B19" s="91" t="n">
-        <v>1</v>
-      </c>
-      <c r="C19" s="84" t="s">
-        <v>67</v>
-      </c>
-      <c r="D19" s="84"/>
-      <c r="E19" s="92" t="n">
-        <v>3305</v>
-      </c>
-      <c r="F19" s="84"/>
-      <c r="G19" s="84" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="90" t="n">
-        <v>43657</v>
-      </c>
-      <c r="B20" s="91" t="n">
+      <c r="B26" s="105" t="n">
         <v>2</v>
       </c>
-      <c r="C20" s="84" t="s">
-        <v>68</v>
-      </c>
-      <c r="D20" s="84"/>
-      <c r="E20" s="92" t="n">
-        <v>1232</v>
-      </c>
-      <c r="F20" s="84"/>
-      <c r="G20" s="84" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="90" t="n">
-        <v>43784</v>
-      </c>
-      <c r="B21" s="91" t="n">
-        <v>1</v>
-      </c>
-      <c r="C21" s="84" t="s">
-        <v>69</v>
-      </c>
-      <c r="D21" s="84"/>
-      <c r="E21" s="92" t="n">
-        <v>4720</v>
-      </c>
-      <c r="F21" s="84"/>
-      <c r="G21" s="84" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="90" t="n">
-        <v>43789</v>
-      </c>
-      <c r="B22" s="91" t="n">
+      <c r="C26" s="98" t="s">
+        <v>76</v>
+      </c>
+      <c r="D26" s="98"/>
+      <c r="E26" s="106" t="n">
+        <v>790</v>
+      </c>
+      <c r="F26" s="98"/>
+      <c r="G26" s="98" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="104" t="n">
+        <v>43804</v>
+      </c>
+      <c r="B27" s="105" t="n">
         <v>2</v>
       </c>
-      <c r="C22" s="84" t="s">
-        <v>70</v>
-      </c>
-      <c r="D22" s="84"/>
-      <c r="E22" s="92" t="n">
-        <v>350</v>
-      </c>
-      <c r="F22" s="84"/>
-      <c r="G22" s="84" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="90" t="n">
-        <v>43789</v>
-      </c>
-      <c r="B23" s="91" t="n">
-        <v>18</v>
-      </c>
-      <c r="C23" s="84" t="s">
-        <v>71</v>
-      </c>
-      <c r="D23" s="84"/>
-      <c r="E23" s="92" t="n">
-        <v>7640</v>
-      </c>
-      <c r="F23" s="84"/>
-      <c r="G23" s="84" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="90" t="n">
-        <v>43791</v>
-      </c>
-      <c r="B24" s="91" t="n">
-        <v>12</v>
-      </c>
-      <c r="C24" s="84" t="s">
-        <v>72</v>
-      </c>
-      <c r="D24" s="84"/>
-      <c r="E24" s="92" t="n">
-        <v>846.48</v>
-      </c>
-      <c r="F24" s="84"/>
-      <c r="G24" s="84" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="90" t="n">
-        <v>43795</v>
-      </c>
-      <c r="B25" s="91" t="n">
+      <c r="C27" s="98" t="s">
+        <v>78</v>
+      </c>
+      <c r="D27" s="98"/>
+      <c r="E27" s="106" t="n">
+        <v>210</v>
+      </c>
+      <c r="F27" s="98"/>
+      <c r="G27" s="98" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="104" t="n">
+        <v>43804</v>
+      </c>
+      <c r="B28" s="105" t="n">
         <v>4</v>
       </c>
-      <c r="C25" s="84" t="s">
-        <v>74</v>
-      </c>
-      <c r="D25" s="84"/>
-      <c r="E25" s="92" t="n">
-        <v>940</v>
-      </c>
-      <c r="F25" s="84"/>
-      <c r="G25" s="84" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="90" t="n">
-        <v>43804</v>
-      </c>
-      <c r="B26" s="91" t="n">
-        <v>2</v>
-      </c>
-      <c r="C26" s="84" t="s">
-        <v>75</v>
-      </c>
-      <c r="D26" s="84"/>
-      <c r="E26" s="92" t="n">
-        <v>790</v>
-      </c>
-      <c r="F26" s="84"/>
-      <c r="G26" s="84" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="90" t="n">
-        <v>43804</v>
-      </c>
-      <c r="B27" s="91" t="n">
-        <v>2</v>
-      </c>
-      <c r="C27" s="84" t="s">
-        <v>77</v>
-      </c>
-      <c r="D27" s="84"/>
-      <c r="E27" s="92" t="n">
-        <v>210</v>
-      </c>
-      <c r="F27" s="84"/>
-      <c r="G27" s="84" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="90" t="n">
-        <v>43804</v>
-      </c>
-      <c r="B28" s="91" t="n">
-        <v>4</v>
-      </c>
-      <c r="C28" s="84" t="s">
-        <v>78</v>
-      </c>
-      <c r="D28" s="84"/>
-      <c r="E28" s="92" t="n">
+      <c r="C28" s="98" t="s">
+        <v>79</v>
+      </c>
+      <c r="D28" s="98"/>
+      <c r="E28" s="106" t="n">
         <v>1160</v>
       </c>
-      <c r="F28" s="84"/>
-      <c r="G28" s="84" t="s">
-        <v>54</v>
+      <c r="F28" s="98"/>
+      <c r="G28" s="98" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="94"/>
-      <c r="B29" s="84"/>
-      <c r="C29" s="84"/>
-      <c r="D29" s="84"/>
-      <c r="E29" s="95" t="n">
+      <c r="A29" s="108"/>
+      <c r="B29" s="98"/>
+      <c r="C29" s="98"/>
+      <c r="D29" s="98"/>
+      <c r="E29" s="109" t="n">
         <v>47426.48</v>
       </c>
-      <c r="F29" s="84" t="s">
-        <v>79</v>
-      </c>
-      <c r="G29" s="96" t="s">
-        <v>79</v>
+      <c r="F29" s="98" t="s">
+        <v>80</v>
+      </c>
+      <c r="G29" s="110" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="94"/>
-      <c r="B30" s="84"/>
-      <c r="C30" s="84"/>
-      <c r="D30" s="84"/>
-      <c r="E30" s="97"/>
-      <c r="F30" s="84"/>
-      <c r="G30" s="84"/>
+      <c r="A30" s="108"/>
+      <c r="B30" s="98"/>
+      <c r="C30" s="98"/>
+      <c r="D30" s="98"/>
+      <c r="E30" s="106"/>
+      <c r="F30" s="98"/>
+      <c r="G30" s="98"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="94"/>
-      <c r="B31" s="84"/>
-      <c r="C31" s="84"/>
-      <c r="D31" s="84"/>
-      <c r="E31" s="84"/>
-      <c r="F31" s="84"/>
-      <c r="G31" s="84"/>
+      <c r="A31" s="108"/>
+      <c r="B31" s="98"/>
+      <c r="C31" s="98"/>
+      <c r="D31" s="98"/>
+      <c r="E31" s="98"/>
+      <c r="F31" s="98"/>
+      <c r="G31" s="98"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="94"/>
-      <c r="B32" s="84"/>
-      <c r="C32" s="84"/>
-      <c r="D32" s="84"/>
-      <c r="E32" s="84"/>
-      <c r="F32" s="84"/>
-      <c r="G32" s="84"/>
+      <c r="A32" s="108"/>
+      <c r="B32" s="98"/>
+      <c r="C32" s="98"/>
+      <c r="D32" s="98"/>
+      <c r="E32" s="98"/>
+      <c r="F32" s="98"/>
+      <c r="G32" s="98"/>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="94"/>
+      <c r="A33" s="108"/>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="94"/>
+      <c r="A34" s="108"/>
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="94"/>
+      <c r="A35" s="108"/>
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="94"/>
+      <c r="A36" s="108"/>
     </row>
     <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="94"/>
+      <c r="A37" s="108"/>
     </row>
     <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="94"/>
+      <c r="A38" s="108"/>
     </row>
     <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="94"/>
+      <c r="A39" s="108"/>
     </row>
     <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="94"/>
+      <c r="A40" s="108"/>
     </row>
     <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="94"/>
+      <c r="A41" s="108"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2548,566 +2684,566 @@
   <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J14" activeCellId="0" sqref="J14"/>
+      <selection pane="topLeft" activeCell="J14" activeCellId="1" sqref="D15:G15 J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.609375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.59375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.87"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="83" t="s">
-        <v>44</v>
-      </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
-      <c r="F1" s="84"/>
-      <c r="G1" s="84"/>
+      <c r="A1" s="97" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="98"/>
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="98"/>
+      <c r="G1" s="98"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="83" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
+      <c r="A2" s="97" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="83" t="s">
-        <v>46</v>
-      </c>
-      <c r="B3" s="84"/>
-      <c r="C3" s="84"/>
-      <c r="D3" s="84"/>
-      <c r="E3" s="84"/>
-      <c r="F3" s="84"/>
-      <c r="G3" s="84"/>
+      <c r="A3" s="97" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="98"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="83" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" s="84"/>
-      <c r="C4" s="84"/>
-      <c r="D4" s="84"/>
-      <c r="E4" s="84"/>
-      <c r="F4" s="84"/>
-      <c r="G4" s="84"/>
+      <c r="A4" s="97" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="98"/>
+      <c r="C4" s="98"/>
+      <c r="D4" s="98"/>
+      <c r="E4" s="98"/>
+      <c r="F4" s="98"/>
+      <c r="G4" s="98"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="98" t="s">
-        <v>48</v>
-      </c>
-      <c r="B6" s="98" t="s">
+      <c r="A6" s="111" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="111" t="s">
+        <v>81</v>
+      </c>
+      <c r="C6" s="111" t="s">
+        <v>82</v>
+      </c>
+      <c r="D6" s="111" t="s">
+        <v>83</v>
+      </c>
+      <c r="E6" s="111" t="s">
+        <v>84</v>
+      </c>
+      <c r="F6" s="100"/>
+      <c r="G6" s="100"/>
+    </row>
+    <row r="7" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="112" t="n">
+        <v>43938</v>
+      </c>
+      <c r="B7" s="113" t="n">
+        <v>849</v>
+      </c>
+      <c r="C7" s="105" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7" s="114" t="s">
+        <v>86</v>
+      </c>
+      <c r="E7" s="115" t="n">
+        <v>1344</v>
+      </c>
+      <c r="F7" s="110"/>
+      <c r="G7" s="98"/>
+    </row>
+    <row r="8" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="112" t="n">
+        <v>43939</v>
+      </c>
+      <c r="B8" s="113" t="n">
+        <v>854</v>
+      </c>
+      <c r="C8" s="105" t="s">
+        <v>85</v>
+      </c>
+      <c r="D8" s="114" t="s">
+        <v>86</v>
+      </c>
+      <c r="E8" s="115" t="n">
+        <v>3305</v>
+      </c>
+      <c r="F8" s="110"/>
+      <c r="G8" s="98"/>
+    </row>
+    <row r="9" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="112" t="n">
+        <v>43979</v>
+      </c>
+      <c r="B9" s="113" t="n">
+        <v>870</v>
+      </c>
+      <c r="C9" s="105" t="s">
+        <v>85</v>
+      </c>
+      <c r="D9" s="114" t="s">
+        <v>86</v>
+      </c>
+      <c r="E9" s="115" t="n">
+        <v>945</v>
+      </c>
+      <c r="F9" s="110"/>
+      <c r="G9" s="98"/>
+    </row>
+    <row r="10" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="112" t="n">
+        <v>44100</v>
+      </c>
+      <c r="B10" s="113" t="n">
+        <v>969</v>
+      </c>
+      <c r="C10" s="105" t="s">
+        <v>85</v>
+      </c>
+      <c r="D10" s="114" t="s">
+        <v>86</v>
+      </c>
+      <c r="E10" s="115" t="n">
+        <v>1010</v>
+      </c>
+      <c r="F10" s="110"/>
+      <c r="G10" s="98"/>
+    </row>
+    <row r="11" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="112" t="n">
+        <v>44036</v>
+      </c>
+      <c r="B11" s="113" t="n">
+        <v>929</v>
+      </c>
+      <c r="C11" s="105" t="s">
+        <v>85</v>
+      </c>
+      <c r="D11" s="114" t="s">
+        <v>86</v>
+      </c>
+      <c r="E11" s="115" t="n">
+        <v>3905</v>
+      </c>
+      <c r="F11" s="110"/>
+      <c r="G11" s="98"/>
+    </row>
+    <row r="12" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="112" t="n">
+        <v>44036</v>
+      </c>
+      <c r="B12" s="113" t="n">
+        <v>926</v>
+      </c>
+      <c r="C12" s="105" t="s">
+        <v>85</v>
+      </c>
+      <c r="D12" s="114" t="s">
+        <v>86</v>
+      </c>
+      <c r="E12" s="115" t="n">
+        <v>2055</v>
+      </c>
+      <c r="F12" s="110"/>
+      <c r="G12" s="98"/>
+    </row>
+    <row r="13" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="112" t="n">
+        <v>44017</v>
+      </c>
+      <c r="B13" s="113" t="n">
+        <v>914</v>
+      </c>
+      <c r="C13" s="105" t="s">
+        <v>85</v>
+      </c>
+      <c r="D13" s="114" t="s">
+        <v>86</v>
+      </c>
+      <c r="E13" s="115" t="n">
+        <v>4700</v>
+      </c>
+      <c r="F13" s="110"/>
+      <c r="G13" s="98"/>
+    </row>
+    <row r="14" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="112" t="n">
+        <v>44108</v>
+      </c>
+      <c r="B14" s="113" t="n">
+        <v>154</v>
+      </c>
+      <c r="C14" s="105" t="s">
+        <v>87</v>
+      </c>
+      <c r="D14" s="114" t="s">
+        <v>88</v>
+      </c>
+      <c r="E14" s="115" t="n">
+        <v>660</v>
+      </c>
+      <c r="F14" s="110"/>
+      <c r="G14" s="98"/>
+    </row>
+    <row r="15" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="112" t="n">
+        <v>44170</v>
+      </c>
+      <c r="B15" s="113" t="n">
+        <v>191</v>
+      </c>
+      <c r="C15" s="105" t="s">
+        <v>87</v>
+      </c>
+      <c r="D15" s="114" t="s">
+        <v>88</v>
+      </c>
+      <c r="E15" s="115" t="n">
+        <v>2740</v>
+      </c>
+      <c r="F15" s="110"/>
+      <c r="G15" s="98"/>
+    </row>
+    <row r="16" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="112" t="n">
+        <v>44118</v>
+      </c>
+      <c r="B16" s="113" t="n">
+        <v>550</v>
+      </c>
+      <c r="C16" s="105" t="s">
+        <v>89</v>
+      </c>
+      <c r="D16" s="114" t="s">
+        <v>90</v>
+      </c>
+      <c r="E16" s="115" t="n">
+        <v>2441</v>
+      </c>
+      <c r="F16" s="110"/>
+      <c r="G16" s="98"/>
+    </row>
+    <row r="17" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="112" t="n">
+        <v>44118</v>
+      </c>
+      <c r="B17" s="113" t="n">
+        <v>551</v>
+      </c>
+      <c r="C17" s="105" t="s">
+        <v>89</v>
+      </c>
+      <c r="D17" s="114" t="s">
+        <v>90</v>
+      </c>
+      <c r="E17" s="115" t="n">
+        <v>3069</v>
+      </c>
+      <c r="F17" s="110"/>
+      <c r="G17" s="98"/>
+      <c r="H17" s="98"/>
+      <c r="I17" s="98"/>
+    </row>
+    <row r="18" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="112" t="n">
+        <v>44155</v>
+      </c>
+      <c r="B18" s="113" t="n">
+        <v>558</v>
+      </c>
+      <c r="C18" s="105" t="s">
+        <v>89</v>
+      </c>
+      <c r="D18" s="114" t="s">
+        <v>90</v>
+      </c>
+      <c r="E18" s="115" t="n">
+        <v>7640</v>
+      </c>
+      <c r="F18" s="110"/>
+      <c r="G18" s="98"/>
+      <c r="H18" s="98"/>
+      <c r="I18" s="98"/>
+    </row>
+    <row r="19" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="112" t="n">
+        <v>44150</v>
+      </c>
+      <c r="B19" s="113" t="n">
+        <v>557</v>
+      </c>
+      <c r="C19" s="105" t="s">
+        <v>89</v>
+      </c>
+      <c r="D19" s="114" t="s">
+        <v>90</v>
+      </c>
+      <c r="E19" s="115" t="n">
+        <v>4720</v>
+      </c>
+      <c r="F19" s="110"/>
+      <c r="G19" s="98"/>
+      <c r="H19" s="98"/>
+      <c r="I19" s="98"/>
+    </row>
+    <row r="20" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="112" t="n">
+        <v>44092</v>
+      </c>
+      <c r="B20" s="113" t="n">
+        <v>548</v>
+      </c>
+      <c r="C20" s="105" t="s">
+        <v>89</v>
+      </c>
+      <c r="D20" s="114" t="s">
+        <v>90</v>
+      </c>
+      <c r="E20" s="115" t="n">
+        <v>5524</v>
+      </c>
+      <c r="F20" s="110"/>
+      <c r="G20" s="98"/>
+      <c r="H20" s="98"/>
+      <c r="I20" s="98"/>
+    </row>
+    <row r="21" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="112" t="n">
+        <v>44161</v>
+      </c>
+      <c r="B21" s="113" t="n">
+        <v>8274</v>
+      </c>
+      <c r="C21" s="105" t="s">
+        <v>91</v>
+      </c>
+      <c r="D21" s="114" t="s">
+        <v>92</v>
+      </c>
+      <c r="E21" s="115" t="n">
+        <v>940</v>
+      </c>
+      <c r="F21" s="110"/>
+      <c r="G21" s="98"/>
+      <c r="H21" s="98"/>
+      <c r="I21" s="98"/>
+    </row>
+    <row r="22" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="112" t="n">
+        <v>44155</v>
+      </c>
+      <c r="B22" s="113" t="n">
+        <v>8267</v>
+      </c>
+      <c r="C22" s="105" t="s">
+        <v>91</v>
+      </c>
+      <c r="D22" s="114" t="s">
+        <v>92</v>
+      </c>
+      <c r="E22" s="115" t="n">
+        <v>350</v>
+      </c>
+      <c r="F22" s="110"/>
+      <c r="G22" s="98"/>
+      <c r="H22" s="98"/>
+      <c r="I22" s="98"/>
+    </row>
+    <row r="23" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="112" t="n">
+        <v>44157</v>
+      </c>
+      <c r="B23" s="113" t="n">
+        <v>1504</v>
+      </c>
+      <c r="C23" s="105" t="s">
+        <v>93</v>
+      </c>
+      <c r="D23" s="114" t="s">
+        <v>94</v>
+      </c>
+      <c r="E23" s="115" t="n">
+        <v>846.48</v>
+      </c>
+      <c r="F23" s="110"/>
+      <c r="G23" s="98"/>
+      <c r="H23" s="98"/>
+      <c r="I23" s="98"/>
+    </row>
+    <row r="24" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="116" t="n">
+        <v>44023</v>
+      </c>
+      <c r="B24" s="113" t="n">
+        <v>5565</v>
+      </c>
+      <c r="C24" s="105" t="s">
+        <v>95</v>
+      </c>
+      <c r="D24" s="114" t="s">
+        <v>96</v>
+      </c>
+      <c r="E24" s="115" t="n">
+        <v>1232</v>
+      </c>
+      <c r="F24" s="110"/>
+      <c r="G24" s="98"/>
+      <c r="H24" s="98"/>
+      <c r="I24" s="98"/>
+    </row>
+    <row r="25" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="98"/>
+      <c r="B25" s="98"/>
+      <c r="C25" s="113" t="s">
+        <v>97</v>
+      </c>
+      <c r="D25" s="113"/>
+      <c r="E25" s="117" t="n">
+        <v>47426.48</v>
+      </c>
+      <c r="F25" s="110" t="s">
         <v>80</v>
       </c>
-      <c r="C6" s="98" t="s">
-        <v>81</v>
-      </c>
-      <c r="D6" s="98" t="s">
-        <v>82</v>
-      </c>
-      <c r="E6" s="98" t="s">
-        <v>83</v>
-      </c>
-      <c r="F6" s="86"/>
-      <c r="G6" s="86"/>
-    </row>
-    <row r="7" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="99" t="n">
-        <v>43938</v>
-      </c>
-      <c r="B7" s="100" t="n">
-        <v>849</v>
-      </c>
-      <c r="C7" s="91" t="s">
-        <v>84</v>
-      </c>
-      <c r="D7" s="101" t="s">
-        <v>85</v>
-      </c>
-      <c r="E7" s="102" t="n">
-        <v>1344</v>
-      </c>
-      <c r="F7" s="96"/>
-      <c r="G7" s="84"/>
-    </row>
-    <row r="8" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="99" t="n">
-        <v>43939</v>
-      </c>
-      <c r="B8" s="100" t="n">
-        <v>854</v>
-      </c>
-      <c r="C8" s="91" t="s">
-        <v>84</v>
-      </c>
-      <c r="D8" s="101" t="s">
-        <v>85</v>
-      </c>
-      <c r="E8" s="102" t="n">
-        <v>3305</v>
-      </c>
-      <c r="F8" s="96"/>
-      <c r="G8" s="84"/>
-    </row>
-    <row r="9" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="99" t="n">
-        <v>43979</v>
-      </c>
-      <c r="B9" s="100" t="n">
-        <v>870</v>
-      </c>
-      <c r="C9" s="91" t="s">
-        <v>84</v>
-      </c>
-      <c r="D9" s="101" t="s">
-        <v>85</v>
-      </c>
-      <c r="E9" s="102" t="n">
-        <v>945</v>
-      </c>
-      <c r="F9" s="96"/>
-      <c r="G9" s="84"/>
-    </row>
-    <row r="10" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="99" t="n">
-        <v>44100</v>
-      </c>
-      <c r="B10" s="100" t="n">
-        <v>969</v>
-      </c>
-      <c r="C10" s="91" t="s">
-        <v>84</v>
-      </c>
-      <c r="D10" s="101" t="s">
-        <v>85</v>
-      </c>
-      <c r="E10" s="102" t="n">
-        <v>1010</v>
-      </c>
-      <c r="F10" s="96"/>
-      <c r="G10" s="84"/>
-    </row>
-    <row r="11" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="99" t="n">
-        <v>44036</v>
-      </c>
-      <c r="B11" s="100" t="n">
-        <v>929</v>
-      </c>
-      <c r="C11" s="91" t="s">
-        <v>84</v>
-      </c>
-      <c r="D11" s="101" t="s">
-        <v>85</v>
-      </c>
-      <c r="E11" s="102" t="n">
-        <v>3905</v>
-      </c>
-      <c r="F11" s="96"/>
-      <c r="G11" s="84"/>
-    </row>
-    <row r="12" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="99" t="n">
-        <v>44036</v>
-      </c>
-      <c r="B12" s="100" t="n">
-        <v>926</v>
-      </c>
-      <c r="C12" s="91" t="s">
-        <v>84</v>
-      </c>
-      <c r="D12" s="101" t="s">
-        <v>85</v>
-      </c>
-      <c r="E12" s="102" t="n">
-        <v>2055</v>
-      </c>
-      <c r="F12" s="96"/>
-      <c r="G12" s="84"/>
-    </row>
-    <row r="13" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="99" t="n">
-        <v>44017</v>
-      </c>
-      <c r="B13" s="100" t="n">
-        <v>914</v>
-      </c>
-      <c r="C13" s="91" t="s">
-        <v>84</v>
-      </c>
-      <c r="D13" s="101" t="s">
-        <v>85</v>
-      </c>
-      <c r="E13" s="102" t="n">
-        <v>4700</v>
-      </c>
-      <c r="F13" s="96"/>
-      <c r="G13" s="84"/>
-    </row>
-    <row r="14" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="99" t="n">
-        <v>44108</v>
-      </c>
-      <c r="B14" s="100" t="n">
-        <v>154</v>
-      </c>
-      <c r="C14" s="91" t="s">
-        <v>86</v>
-      </c>
-      <c r="D14" s="101" t="s">
-        <v>87</v>
-      </c>
-      <c r="E14" s="102" t="n">
-        <v>660</v>
-      </c>
-      <c r="F14" s="96"/>
-      <c r="G14" s="84"/>
-    </row>
-    <row r="15" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="99" t="n">
-        <v>44170</v>
-      </c>
-      <c r="B15" s="100" t="n">
-        <v>191</v>
-      </c>
-      <c r="C15" s="91" t="s">
-        <v>86</v>
-      </c>
-      <c r="D15" s="101" t="s">
-        <v>87</v>
-      </c>
-      <c r="E15" s="102" t="n">
-        <v>2740</v>
-      </c>
-      <c r="F15" s="96"/>
-      <c r="G15" s="84"/>
-    </row>
-    <row r="16" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="99" t="n">
-        <v>44118</v>
-      </c>
-      <c r="B16" s="100" t="n">
-        <v>550</v>
-      </c>
-      <c r="C16" s="91" t="s">
-        <v>88</v>
-      </c>
-      <c r="D16" s="101" t="s">
-        <v>89</v>
-      </c>
-      <c r="E16" s="102" t="n">
-        <v>2441</v>
-      </c>
-      <c r="F16" s="96"/>
-      <c r="G16" s="84"/>
-    </row>
-    <row r="17" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="99" t="n">
-        <v>44118</v>
-      </c>
-      <c r="B17" s="100" t="n">
-        <v>551</v>
-      </c>
-      <c r="C17" s="91" t="s">
-        <v>88</v>
-      </c>
-      <c r="D17" s="101" t="s">
-        <v>89</v>
-      </c>
-      <c r="E17" s="102" t="n">
-        <v>3069</v>
-      </c>
-      <c r="F17" s="96"/>
-      <c r="G17" s="84"/>
-      <c r="H17" s="84"/>
-      <c r="I17" s="84"/>
-    </row>
-    <row r="18" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="99" t="n">
-        <v>44155</v>
-      </c>
-      <c r="B18" s="100" t="n">
-        <v>558</v>
-      </c>
-      <c r="C18" s="91" t="s">
-        <v>88</v>
-      </c>
-      <c r="D18" s="101" t="s">
-        <v>89</v>
-      </c>
-      <c r="E18" s="102" t="n">
-        <v>7640</v>
-      </c>
-      <c r="F18" s="96"/>
-      <c r="G18" s="84"/>
-      <c r="H18" s="84"/>
-      <c r="I18" s="84"/>
-    </row>
-    <row r="19" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="99" t="n">
-        <v>44150</v>
-      </c>
-      <c r="B19" s="100" t="n">
-        <v>557</v>
-      </c>
-      <c r="C19" s="91" t="s">
-        <v>88</v>
-      </c>
-      <c r="D19" s="101" t="s">
-        <v>89</v>
-      </c>
-      <c r="E19" s="102" t="n">
-        <v>4720</v>
-      </c>
-      <c r="F19" s="96"/>
-      <c r="G19" s="84"/>
-      <c r="H19" s="84"/>
-      <c r="I19" s="84"/>
-    </row>
-    <row r="20" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="99" t="n">
-        <v>44092</v>
-      </c>
-      <c r="B20" s="100" t="n">
-        <v>548</v>
-      </c>
-      <c r="C20" s="91" t="s">
-        <v>88</v>
-      </c>
-      <c r="D20" s="101" t="s">
-        <v>89</v>
-      </c>
-      <c r="E20" s="102" t="n">
-        <v>5524</v>
-      </c>
-      <c r="F20" s="96"/>
-      <c r="G20" s="84"/>
-      <c r="H20" s="84"/>
-      <c r="I20" s="84"/>
-    </row>
-    <row r="21" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="99" t="n">
-        <v>44161</v>
-      </c>
-      <c r="B21" s="100" t="n">
-        <v>8274</v>
-      </c>
-      <c r="C21" s="91" t="s">
-        <v>90</v>
-      </c>
-      <c r="D21" s="101" t="s">
-        <v>91</v>
-      </c>
-      <c r="E21" s="102" t="n">
-        <v>940</v>
-      </c>
-      <c r="F21" s="96"/>
-      <c r="G21" s="84"/>
-      <c r="H21" s="84"/>
-      <c r="I21" s="84"/>
-    </row>
-    <row r="22" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="99" t="n">
-        <v>44155</v>
-      </c>
-      <c r="B22" s="100" t="n">
-        <v>8267</v>
-      </c>
-      <c r="C22" s="91" t="s">
-        <v>90</v>
-      </c>
-      <c r="D22" s="101" t="s">
-        <v>91</v>
-      </c>
-      <c r="E22" s="102" t="n">
-        <v>350</v>
-      </c>
-      <c r="F22" s="96"/>
-      <c r="G22" s="84"/>
-      <c r="H22" s="84"/>
-      <c r="I22" s="84"/>
-    </row>
-    <row r="23" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="99" t="n">
-        <v>44157</v>
-      </c>
-      <c r="B23" s="100" t="n">
-        <v>1504</v>
-      </c>
-      <c r="C23" s="91" t="s">
-        <v>92</v>
-      </c>
-      <c r="D23" s="101" t="s">
-        <v>93</v>
-      </c>
-      <c r="E23" s="102" t="n">
-        <v>846.48</v>
-      </c>
-      <c r="F23" s="96"/>
-      <c r="G23" s="84"/>
-      <c r="H23" s="84"/>
-      <c r="I23" s="84"/>
-    </row>
-    <row r="24" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="103" t="n">
-        <v>44023</v>
-      </c>
-      <c r="B24" s="100" t="n">
-        <v>5565</v>
-      </c>
-      <c r="C24" s="91" t="s">
-        <v>94</v>
-      </c>
-      <c r="D24" s="101" t="s">
-        <v>95</v>
-      </c>
-      <c r="E24" s="102" t="n">
-        <v>1232</v>
-      </c>
-      <c r="F24" s="96"/>
-      <c r="G24" s="84"/>
-      <c r="H24" s="84"/>
-      <c r="I24" s="84"/>
-    </row>
-    <row r="25" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="84"/>
-      <c r="B25" s="84"/>
-      <c r="C25" s="100" t="s">
-        <v>96</v>
-      </c>
-      <c r="D25" s="100"/>
-      <c r="E25" s="104" t="n">
-        <v>47426.48</v>
-      </c>
-      <c r="F25" s="96" t="s">
-        <v>79</v>
-      </c>
-      <c r="G25" s="96" t="s">
-        <v>79</v>
-      </c>
-      <c r="H25" s="96" t="s">
-        <v>79</v>
-      </c>
-      <c r="I25" s="84"/>
+      <c r="G25" s="110" t="s">
+        <v>80</v>
+      </c>
+      <c r="H25" s="110" t="s">
+        <v>80</v>
+      </c>
+      <c r="I25" s="98"/>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="84"/>
-      <c r="B26" s="84"/>
-      <c r="C26" s="84"/>
-      <c r="D26" s="84"/>
-      <c r="E26" s="96"/>
-      <c r="F26" s="86"/>
-      <c r="G26" s="86"/>
-      <c r="H26" s="84"/>
-      <c r="I26" s="84"/>
+      <c r="A26" s="98"/>
+      <c r="B26" s="98"/>
+      <c r="C26" s="98"/>
+      <c r="D26" s="98"/>
+      <c r="E26" s="110"/>
+      <c r="F26" s="100"/>
+      <c r="G26" s="100"/>
+      <c r="H26" s="98"/>
+      <c r="I26" s="98"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="84"/>
-      <c r="B27" s="84"/>
-      <c r="C27" s="84"/>
-      <c r="D27" s="84"/>
-      <c r="E27" s="105"/>
-      <c r="F27" s="84"/>
-      <c r="G27" s="84"/>
-      <c r="H27" s="84"/>
-      <c r="I27" s="84"/>
+      <c r="A27" s="98"/>
+      <c r="B27" s="98"/>
+      <c r="C27" s="98"/>
+      <c r="D27" s="98"/>
+      <c r="E27" s="98"/>
+      <c r="F27" s="98"/>
+      <c r="G27" s="98"/>
+      <c r="H27" s="98"/>
+      <c r="I27" s="98"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="84"/>
-      <c r="B28" s="84"/>
-      <c r="C28" s="84"/>
-      <c r="D28" s="84"/>
-      <c r="E28" s="105"/>
-      <c r="F28" s="84"/>
-      <c r="G28" s="84"/>
-      <c r="H28" s="84"/>
-      <c r="I28" s="84"/>
+      <c r="A28" s="98"/>
+      <c r="B28" s="98"/>
+      <c r="C28" s="98"/>
+      <c r="D28" s="98"/>
+      <c r="E28" s="98"/>
+      <c r="F28" s="98"/>
+      <c r="G28" s="98"/>
+      <c r="H28" s="98"/>
+      <c r="I28" s="98"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="84"/>
-      <c r="B29" s="84"/>
-      <c r="C29" s="84"/>
-      <c r="D29" s="84"/>
-      <c r="E29" s="105"/>
-      <c r="F29" s="84"/>
-      <c r="G29" s="84"/>
-      <c r="H29" s="84"/>
-      <c r="I29" s="84"/>
+      <c r="A29" s="98"/>
+      <c r="B29" s="98"/>
+      <c r="C29" s="98"/>
+      <c r="D29" s="98"/>
+      <c r="E29" s="98"/>
+      <c r="F29" s="98"/>
+      <c r="G29" s="98"/>
+      <c r="H29" s="98"/>
+      <c r="I29" s="98"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="84"/>
-      <c r="B30" s="84"/>
-      <c r="C30" s="84"/>
-      <c r="D30" s="84"/>
-      <c r="E30" s="105"/>
-      <c r="F30" s="84"/>
-      <c r="G30" s="84"/>
-      <c r="H30" s="84"/>
-      <c r="I30" s="84"/>
+      <c r="A30" s="98"/>
+      <c r="B30" s="98"/>
+      <c r="C30" s="98"/>
+      <c r="D30" s="98"/>
+      <c r="E30" s="98"/>
+      <c r="F30" s="98"/>
+      <c r="G30" s="98"/>
+      <c r="H30" s="98"/>
+      <c r="I30" s="98"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="84"/>
-      <c r="B31" s="84"/>
-      <c r="C31" s="84"/>
-      <c r="D31" s="84"/>
-      <c r="E31" s="105" t="s">
-        <v>79</v>
-      </c>
-      <c r="F31" s="84"/>
-      <c r="G31" s="84"/>
-      <c r="H31" s="84"/>
-      <c r="I31" s="96" t="s">
-        <v>79</v>
+      <c r="A31" s="98"/>
+      <c r="B31" s="98"/>
+      <c r="C31" s="98"/>
+      <c r="D31" s="98"/>
+      <c r="E31" s="98" t="s">
+        <v>80</v>
+      </c>
+      <c r="F31" s="98"/>
+      <c r="G31" s="98"/>
+      <c r="H31" s="98"/>
+      <c r="I31" s="110" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="84"/>
-      <c r="B32" s="84"/>
-      <c r="C32" s="84"/>
-      <c r="D32" s="84"/>
-      <c r="E32" s="105"/>
-      <c r="F32" s="84"/>
-      <c r="G32" s="84"/>
-      <c r="H32" s="84"/>
-      <c r="I32" s="84"/>
+      <c r="A32" s="98"/>
+      <c r="B32" s="98"/>
+      <c r="C32" s="98"/>
+      <c r="D32" s="98"/>
+      <c r="E32" s="98"/>
+      <c r="F32" s="98"/>
+      <c r="G32" s="98"/>
+      <c r="H32" s="98"/>
+      <c r="I32" s="98"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E33" s="105"/>
+      <c r="E33" s="98"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E34" s="106" t="s">
-        <v>79</v>
+      <c r="E34" s="110" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E35" s="106"/>
+      <c r="E35" s="110"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E36" s="96"/>
+      <c r="E36" s="110"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E37" s="96"/>
+      <c r="E37" s="110"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E38" s="96"/>
+      <c r="E38" s="110"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E39" s="96"/>
+      <c r="E39" s="110"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E40" s="96"/>
+      <c r="E40" s="110"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E41" s="96"/>
+      <c r="E41" s="110"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
correcion de cedulas sumarias
</commit_message>
<xml_diff>
--- a/FASE II - Ejecucion/5000 Activos/5400 Inventarios/5401 - Auditoria de Inventarios.xlsx
+++ b/FASE II - Ejecucion/5000 Activos/5400 Inventarios/5401 - Auditoria de Inventarios.xlsx
@@ -10,7 +10,7 @@
   <sheets>
     <sheet name="Cedula Resumen" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Mobiliario" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Hoja2" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Mobiliario2" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="100">
   <si>
     <t xml:space="preserve">Cliente:</t>
   </si>
@@ -123,7 +123,10 @@
     <t xml:space="preserve">Mercaderías en Transito</t>
   </si>
   <si>
-    <t xml:space="preserve">Amortizacion de mobiliario para Eventos ⅓</t>
+    <t xml:space="preserve">Amortización de mobiliario para Eventos ⅓</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1)</t>
   </si>
   <si>
     <t xml:space="preserve">Total</t>
@@ -157,6 +160,9 @@
   </si>
   <si>
     <t xml:space="preserve">Conclusiones (A ser completado por el Auditor a cargo del compromiso):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Este rubro representa el gasto de Amortización del inventario, dicho valor corresponde al 33%, del inventario</t>
   </si>
   <si>
     <t xml:space="preserve">VISACOM S.A.</t>
@@ -337,7 +343,7 @@
     <numFmt numFmtId="175" formatCode="dd\-mmm"/>
     <numFmt numFmtId="176" formatCode="mmm\-yy"/>
   </numFmts>
-  <fonts count="28">
+  <fonts count="29">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -497,6 +503,14 @@
     </font>
     <font>
       <b val="true"/>
+      <sz val="10.5"/>
+      <color rgb="FFFF4000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -543,7 +557,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -602,12 +616,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -894,7 +902,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="119">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1087,15 +1095,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="18" fillId="11" borderId="6" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="170" fontId="22" fillId="10" borderId="6" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="18" fillId="0" borderId="6" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="18" fillId="11" borderId="7" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="170" fontId="18" fillId="0" borderId="7" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="18" fillId="11" borderId="8" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="170" fontId="18" fillId="0" borderId="8" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1283,7 +1295,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="33" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="33" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1295,22 +1307,22 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="33" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="33" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="174" fontId="23" fillId="0" borderId="0" xfId="33" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="33" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="33" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="174" fontId="24" fillId="0" borderId="0" xfId="33" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="33" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="168" fontId="18" fillId="0" borderId="0" xfId="33" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1323,7 +1335,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="33" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="33" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1339,7 +1351,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="33" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="33" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1355,7 +1367,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="174" fontId="27" fillId="0" borderId="0" xfId="33" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="174" fontId="28" fillId="0" borderId="0" xfId="33" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1363,7 +1375,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="174" fontId="27" fillId="0" borderId="26" xfId="33" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="174" fontId="28" fillId="0" borderId="26" xfId="33" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1441,7 +1453,7 @@
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FFFF4000"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
@@ -1462,10 +1474,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M44"/>
+  <dimension ref="A1:M45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15:G15"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1811,22 +1823,24 @@
         <v>-372</v>
       </c>
     </row>
-    <row r="15" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" s="7" customFormat="true" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="38"/>
       <c r="B15" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="21"/>
-      <c r="D15" s="48" t="n">
+      <c r="C15" s="48" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="49" t="n">
         <v>0</v>
       </c>
-      <c r="E15" s="49" t="n">
+      <c r="E15" s="50" t="n">
         <v>0</v>
       </c>
-      <c r="F15" s="50" t="n">
+      <c r="F15" s="51" t="n">
         <v>15808.83</v>
       </c>
-      <c r="G15" s="48" t="n">
+      <c r="G15" s="49" t="n">
         <f aca="false">D15+E15-F15</f>
         <v>-15808.83</v>
       </c>
@@ -1841,8 +1855,8 @@
       </c>
     </row>
     <row r="16" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="51"/>
-      <c r="B16" s="52"/>
+      <c r="A16" s="52"/>
+      <c r="B16" s="53"/>
       <c r="C16" s="21"/>
       <c r="D16" s="34" t="n">
         <v>0</v>
@@ -1853,12 +1867,12 @@
       <c r="F16" s="33" t="n">
         <v>0</v>
       </c>
-      <c r="G16" s="53" t="n">
+      <c r="G16" s="54" t="n">
         <f aca="false">D16+E16-F16</f>
         <v>0</v>
       </c>
-      <c r="H16" s="54"/>
-      <c r="I16" s="55"/>
+      <c r="H16" s="55"/>
+      <c r="I16" s="56"/>
       <c r="J16" s="34" t="n">
         <v>0</v>
       </c>
@@ -1867,210 +1881,218 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" s="61" customFormat="true" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="56"/>
-      <c r="B17" s="57" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="57"/>
-      <c r="D17" s="58" t="n">
+    <row r="17" s="62" customFormat="true" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="57"/>
+      <c r="B17" s="58" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="58"/>
+      <c r="D17" s="59" t="n">
         <f aca="false">SUM(D9:D15)</f>
         <v>47426</v>
       </c>
-      <c r="E17" s="58" t="n">
+      <c r="E17" s="59" t="n">
         <f aca="false">SUM(E9:E15)</f>
         <v>13000</v>
       </c>
-      <c r="F17" s="58" t="n">
+      <c r="F17" s="59" t="n">
         <f aca="false">SUM(F9:F15)</f>
         <v>15808.83</v>
       </c>
-      <c r="G17" s="59" t="n">
+      <c r="G17" s="60" t="n">
         <f aca="false">SUM(G9:G15)</f>
         <v>44617.17</v>
       </c>
-      <c r="H17" s="56"/>
-      <c r="I17" s="56"/>
-      <c r="J17" s="58" t="n">
+      <c r="H17" s="57"/>
+      <c r="I17" s="57"/>
+      <c r="J17" s="59" t="n">
         <f aca="false">SUM(J9:J15)</f>
         <v>61299</v>
       </c>
-      <c r="K17" s="60" t="n">
+      <c r="K17" s="61" t="n">
         <f aca="false">SUM(K9:K15)</f>
         <v>-16681.83</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="62"/>
-      <c r="C20" s="62"/>
-      <c r="D20" s="63" t="s">
-        <v>35</v>
-      </c>
-      <c r="E20" s="64" t="s">
-        <v>35</v>
+      <c r="B20" s="63"/>
+      <c r="C20" s="63"/>
+      <c r="D20" s="64" t="s">
+        <v>36</v>
+      </c>
+      <c r="E20" s="65" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="65" t="s">
-        <v>36</v>
-      </c>
-      <c r="C21" s="66"/>
-      <c r="D21" s="67" t="n">
+      <c r="B21" s="66" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="67"/>
+      <c r="D21" s="68" t="n">
         <v>44196</v>
       </c>
-      <c r="E21" s="67" t="n">
+      <c r="E21" s="68" t="n">
         <v>43830</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="68"/>
-      <c r="C22" s="69"/>
-      <c r="D22" s="70"/>
-      <c r="E22" s="71"/>
+      <c r="B22" s="69"/>
+      <c r="C22" s="70"/>
+      <c r="D22" s="71"/>
+      <c r="E22" s="72"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="68" t="s">
+      <c r="B23" s="69" t="s">
         <v>27</v>
       </c>
-      <c r="C23" s="72"/>
-      <c r="D23" s="73" t="n">
+      <c r="C23" s="73"/>
+      <c r="D23" s="74" t="n">
         <f aca="false">G11</f>
         <v>47426</v>
       </c>
-      <c r="E23" s="74" t="n">
+      <c r="E23" s="75" t="n">
         <f aca="false">J11</f>
         <v>47426</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="68" t="s">
-        <v>37</v>
-      </c>
-      <c r="C24" s="72"/>
-      <c r="D24" s="73" t="n">
+      <c r="B24" s="69" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="73"/>
+      <c r="D24" s="74" t="n">
         <f aca="false">SUM(G12:G14)</f>
         <v>13000</v>
       </c>
-      <c r="E24" s="74" t="n">
+      <c r="E24" s="75" t="n">
         <f aca="false">SUM(J12:J15)</f>
         <v>13873</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="68"/>
-      <c r="C25" s="72"/>
-      <c r="D25" s="75"/>
-      <c r="E25" s="76"/>
+      <c r="B25" s="69"/>
+      <c r="C25" s="73"/>
+      <c r="D25" s="76"/>
+      <c r="E25" s="77"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="66" t="s">
-        <v>34</v>
-      </c>
-      <c r="C26" s="77"/>
-      <c r="D26" s="78" t="n">
+      <c r="B26" s="67" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" s="78"/>
+      <c r="D26" s="79" t="n">
         <f aca="false">+SUM(D23:D24)</f>
         <v>60426</v>
       </c>
-      <c r="E26" s="79" t="n">
+      <c r="E26" s="80" t="n">
         <f aca="false">+SUM(E23:E24)</f>
         <v>61299</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="80"/>
-      <c r="C27" s="80"/>
-      <c r="D27" s="81"/>
-      <c r="E27" s="82"/>
+      <c r="B27" s="81"/>
+      <c r="C27" s="81"/>
+      <c r="D27" s="82"/>
+      <c r="E27" s="83"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="83" t="s">
+      <c r="B28" s="84" t="s">
         <v>33</v>
       </c>
-      <c r="C28" s="84"/>
-      <c r="D28" s="85" t="n">
+      <c r="C28" s="85"/>
+      <c r="D28" s="86" t="n">
         <f aca="false">G15</f>
         <v>-15808.83</v>
       </c>
-      <c r="E28" s="86" t="n">
+      <c r="E28" s="87" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="77"/>
-      <c r="C29" s="77"/>
-      <c r="D29" s="87" t="n">
+      <c r="B29" s="78"/>
+      <c r="C29" s="78"/>
+      <c r="D29" s="88" t="n">
         <f aca="false">D26+D28</f>
         <v>44617.17</v>
       </c>
-      <c r="E29" s="87" t="n">
+      <c r="E29" s="88" t="n">
         <f aca="false">E26+E28</f>
         <v>61299</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="88" t="s">
-        <v>38</v>
-      </c>
-      <c r="B34" s="89"/>
-      <c r="C34" s="89"/>
-      <c r="D34" s="89"/>
-      <c r="E34" s="89"/>
-      <c r="F34" s="89"/>
-      <c r="G34" s="89"/>
-      <c r="H34" s="89"/>
-      <c r="I34" s="90"/>
-      <c r="J34" s="91"/>
-      <c r="K34" s="91"/>
-      <c r="L34" s="92"/>
-      <c r="M34" s="91"/>
+      <c r="A34" s="89" t="s">
+        <v>39</v>
+      </c>
+      <c r="B34" s="90"/>
+      <c r="C34" s="90"/>
+      <c r="D34" s="90"/>
+      <c r="E34" s="90"/>
+      <c r="F34" s="90"/>
+      <c r="G34" s="90"/>
+      <c r="H34" s="90"/>
+      <c r="I34" s="91"/>
+      <c r="J34" s="92"/>
+      <c r="K34" s="92"/>
+      <c r="L34" s="93"/>
+      <c r="M34" s="92"/>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="93" t="s">
-        <v>39</v>
-      </c>
-      <c r="I35" s="94"/>
+      <c r="A35" s="94" t="s">
+        <v>40</v>
+      </c>
+      <c r="I35" s="95"/>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="93"/>
-      <c r="I36" s="94"/>
+      <c r="A36" s="94"/>
+      <c r="I36" s="95"/>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="95" t="s">
-        <v>40</v>
-      </c>
-      <c r="I37" s="94"/>
+      <c r="A37" s="96" t="s">
+        <v>41</v>
+      </c>
+      <c r="I37" s="95"/>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="93" t="s">
-        <v>41</v>
-      </c>
-      <c r="I38" s="94"/>
+      <c r="A38" s="94" t="s">
+        <v>42</v>
+      </c>
+      <c r="I38" s="95"/>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="93" t="s">
-        <v>42</v>
-      </c>
-      <c r="I39" s="94"/>
+      <c r="A39" s="94" t="s">
+        <v>43</v>
+      </c>
+      <c r="I39" s="95"/>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="93"/>
-      <c r="I40" s="94"/>
+      <c r="A40" s="94"/>
+      <c r="I40" s="95"/>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="93"/>
-      <c r="I41" s="94"/>
+      <c r="A41" s="94"/>
+      <c r="I41" s="95"/>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="95" t="s">
-        <v>43</v>
-      </c>
-      <c r="I42" s="94"/>
+      <c r="A42" s="96" t="s">
+        <v>44</v>
+      </c>
+      <c r="I42" s="95"/>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="96" t="s">
-        <v>44</v>
+      <c r="A44" s="97" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="48" t="s">
+        <v>34</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -2109,561 +2131,561 @@
   </sheetPr>
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L29" activeCellId="1" sqref="D15:G15 L29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.59375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.56640625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="97" t="s">
-        <v>45</v>
-      </c>
-      <c r="B1" s="98"/>
-      <c r="C1" s="98"/>
-      <c r="D1" s="98"/>
-      <c r="E1" s="98"/>
-      <c r="F1" s="98"/>
-      <c r="G1" s="98"/>
+      <c r="A1" s="98" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="99"/>
+      <c r="C1" s="99"/>
+      <c r="D1" s="99"/>
+      <c r="E1" s="99"/>
+      <c r="F1" s="99"/>
+      <c r="G1" s="99"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="97" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2" s="98"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
+      <c r="A2" s="98" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="99"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="97" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" s="98"/>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
+      <c r="A3" s="98" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="99"/>
+      <c r="C3" s="99"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="99"/>
+      <c r="G3" s="99"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="97" t="s">
-        <v>48</v>
-      </c>
-      <c r="B4" s="98"/>
-      <c r="C4" s="98"/>
-      <c r="D4" s="98"/>
-      <c r="E4" s="98"/>
-      <c r="F4" s="98"/>
-      <c r="G4" s="98"/>
+      <c r="A4" s="98" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="99"/>
+      <c r="C4" s="99"/>
+      <c r="D4" s="99"/>
+      <c r="E4" s="99"/>
+      <c r="F4" s="99"/>
+      <c r="G4" s="99"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="99" t="s">
-        <v>49</v>
-      </c>
-      <c r="B6" s="100" t="s">
-        <v>50</v>
-      </c>
-      <c r="C6" s="101" t="s">
+      <c r="A6" s="100" t="s">
         <v>51</v>
       </c>
-      <c r="D6" s="98"/>
-      <c r="E6" s="102" t="s">
+      <c r="B6" s="101" t="s">
         <v>52</v>
       </c>
-      <c r="F6" s="98"/>
-      <c r="G6" s="103" t="s">
+      <c r="C6" s="102" t="s">
         <v>53</v>
       </c>
+      <c r="D6" s="99"/>
+      <c r="E6" s="103" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" s="99"/>
+      <c r="G6" s="104" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="104" t="n">
+      <c r="A7" s="105" t="n">
         <v>43572</v>
       </c>
-      <c r="B7" s="105" t="n">
+      <c r="B7" s="106" t="n">
         <v>1</v>
       </c>
-      <c r="C7" s="98" t="s">
-        <v>54</v>
-      </c>
-      <c r="D7" s="98"/>
-      <c r="E7" s="106" t="n">
+      <c r="C7" s="99" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" s="99"/>
+      <c r="E7" s="107" t="n">
         <v>1344</v>
       </c>
-      <c r="F7" s="98"/>
-      <c r="G7" s="98" t="s">
-        <v>55</v>
+      <c r="F7" s="99"/>
+      <c r="G7" s="99" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="104" t="n">
+      <c r="A8" s="105" t="n">
         <v>43651</v>
       </c>
-      <c r="B8" s="105" t="n">
+      <c r="B8" s="106" t="n">
         <v>1</v>
       </c>
-      <c r="C8" s="98" t="s">
-        <v>56</v>
-      </c>
-      <c r="D8" s="98"/>
-      <c r="E8" s="106" t="n">
+      <c r="C8" s="99" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="99"/>
+      <c r="E8" s="107" t="n">
         <v>4700</v>
       </c>
-      <c r="F8" s="98"/>
-      <c r="G8" s="98" t="s">
-        <v>55</v>
+      <c r="F8" s="99"/>
+      <c r="G8" s="99" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="104" t="n">
+      <c r="A9" s="105" t="n">
         <v>43670</v>
       </c>
-      <c r="B9" s="105" t="n">
+      <c r="B9" s="106" t="n">
         <v>1</v>
       </c>
-      <c r="C9" s="98" t="s">
+      <c r="C9" s="99" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" s="99"/>
+      <c r="E9" s="107" t="n">
+        <v>3905</v>
+      </c>
+      <c r="F9" s="99"/>
+      <c r="G9" s="99" t="s">
         <v>57</v>
       </c>
-      <c r="D9" s="98"/>
-      <c r="E9" s="106" t="n">
-        <v>3905</v>
-      </c>
-      <c r="F9" s="98"/>
-      <c r="G9" s="98" t="s">
-        <v>55</v>
-      </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="104" t="n">
+      <c r="A10" s="105" t="n">
         <v>43670</v>
       </c>
-      <c r="B10" s="105" t="n">
+      <c r="B10" s="106" t="n">
         <v>1</v>
       </c>
-      <c r="C10" s="98" t="s">
-        <v>58</v>
-      </c>
-      <c r="D10" s="98"/>
-      <c r="E10" s="106" t="n">
+      <c r="C10" s="99" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="99"/>
+      <c r="E10" s="107" t="n">
         <v>2055</v>
       </c>
-      <c r="F10" s="98"/>
-      <c r="G10" s="98" t="s">
-        <v>55</v>
+      <c r="F10" s="99"/>
+      <c r="G10" s="99" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="104" t="n">
+      <c r="A11" s="105" t="n">
         <v>43726</v>
       </c>
-      <c r="B11" s="105" t="n">
+      <c r="B11" s="106" t="n">
         <v>1</v>
       </c>
-      <c r="C11" s="98" t="s">
-        <v>59</v>
-      </c>
-      <c r="D11" s="98"/>
-      <c r="E11" s="106" t="n">
+      <c r="C11" s="99" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" s="99"/>
+      <c r="E11" s="107" t="n">
         <v>5524</v>
       </c>
-      <c r="F11" s="98"/>
-      <c r="G11" s="98" t="s">
-        <v>60</v>
+      <c r="F11" s="99"/>
+      <c r="G11" s="99" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="104" t="n">
+      <c r="A12" s="105" t="n">
         <v>43734</v>
       </c>
-      <c r="B12" s="105" t="n">
+      <c r="B12" s="106" t="n">
         <v>1</v>
       </c>
-      <c r="C12" s="107" t="s">
-        <v>61</v>
-      </c>
-      <c r="D12" s="98"/>
-      <c r="E12" s="106" t="n">
+      <c r="C12" s="108" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" s="99"/>
+      <c r="E12" s="107" t="n">
         <v>1010</v>
       </c>
-      <c r="F12" s="98"/>
-      <c r="G12" s="98" t="s">
-        <v>55</v>
+      <c r="F12" s="99"/>
+      <c r="G12" s="99" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="104" t="n">
+      <c r="A13" s="105" t="n">
         <v>43742</v>
       </c>
-      <c r="B13" s="105" t="n">
+      <c r="B13" s="106" t="n">
         <v>1</v>
       </c>
-      <c r="C13" s="98" t="s">
+      <c r="C13" s="99" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" s="99"/>
+      <c r="E13" s="107" t="n">
+        <v>660</v>
+      </c>
+      <c r="F13" s="99"/>
+      <c r="G13" s="99" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="105" t="n">
+        <v>43752</v>
+      </c>
+      <c r="B14" s="106" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" s="99" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" s="99"/>
+      <c r="E14" s="107" t="n">
+        <v>2441</v>
+      </c>
+      <c r="F14" s="99"/>
+      <c r="G14" s="99" t="s">
         <v>62</v>
       </c>
-      <c r="D13" s="98"/>
-      <c r="E13" s="106" t="n">
-        <v>660</v>
-      </c>
-      <c r="F13" s="98"/>
-      <c r="G13" s="98" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="104" t="n">
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="105" t="n">
         <v>43752</v>
       </c>
-      <c r="B14" s="105" t="n">
+      <c r="B15" s="106" t="n">
         <v>1</v>
       </c>
-      <c r="C14" s="98" t="s">
-        <v>63</v>
-      </c>
-      <c r="D14" s="98"/>
-      <c r="E14" s="106" t="n">
-        <v>2441</v>
-      </c>
-      <c r="F14" s="98"/>
-      <c r="G14" s="98" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="104" t="n">
-        <v>43752</v>
-      </c>
-      <c r="B15" s="105" t="n">
+      <c r="C15" s="99" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="99"/>
+      <c r="E15" s="107" t="n">
+        <v>3069</v>
+      </c>
+      <c r="F15" s="99"/>
+      <c r="G15" s="99" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="105" t="n">
+        <v>43613</v>
+      </c>
+      <c r="B16" s="106" t="n">
         <v>1</v>
       </c>
-      <c r="C15" s="98" t="s">
-        <v>64</v>
-      </c>
-      <c r="D15" s="98"/>
-      <c r="E15" s="106" t="n">
-        <v>3069</v>
-      </c>
-      <c r="F15" s="98"/>
-      <c r="G15" s="98" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="104" t="n">
+      <c r="C16" s="99" t="s">
+        <v>67</v>
+      </c>
+      <c r="D16" s="99"/>
+      <c r="E16" s="107" t="n">
+        <v>395</v>
+      </c>
+      <c r="F16" s="99"/>
+      <c r="G16" s="99" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="105" t="n">
         <v>43613</v>
       </c>
-      <c r="B16" s="105" t="n">
+      <c r="B17" s="106" t="n">
         <v>1</v>
       </c>
-      <c r="C16" s="98" t="s">
-        <v>65</v>
-      </c>
-      <c r="D16" s="98"/>
-      <c r="E16" s="106" t="n">
-        <v>395</v>
-      </c>
-      <c r="F16" s="98"/>
-      <c r="G16" s="98" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="104" t="n">
-        <v>43613</v>
-      </c>
-      <c r="B17" s="105" t="n">
+      <c r="C17" s="99" t="s">
+        <v>68</v>
+      </c>
+      <c r="D17" s="99"/>
+      <c r="E17" s="107" t="n">
+        <v>550</v>
+      </c>
+      <c r="F17" s="99"/>
+      <c r="G17" s="99" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="105" t="n">
+        <v>43804</v>
+      </c>
+      <c r="B18" s="106" t="n">
         <v>1</v>
       </c>
-      <c r="C17" s="98" t="s">
-        <v>66</v>
-      </c>
-      <c r="D17" s="98"/>
-      <c r="E17" s="106" t="n">
-        <v>550</v>
-      </c>
-      <c r="F17" s="98"/>
-      <c r="G17" s="98" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="104" t="n">
+      <c r="C18" s="99" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" s="99"/>
+      <c r="E18" s="107" t="n">
+        <v>580</v>
+      </c>
+      <c r="F18" s="99"/>
+      <c r="G18" s="99" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="105" t="n">
+        <v>43573</v>
+      </c>
+      <c r="B19" s="106" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" s="99" t="s">
+        <v>70</v>
+      </c>
+      <c r="D19" s="99"/>
+      <c r="E19" s="107" t="n">
+        <v>3305</v>
+      </c>
+      <c r="F19" s="99"/>
+      <c r="G19" s="99" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="105" t="n">
+        <v>43657</v>
+      </c>
+      <c r="B20" s="106" t="n">
+        <v>2</v>
+      </c>
+      <c r="C20" s="99" t="s">
+        <v>71</v>
+      </c>
+      <c r="D20" s="99"/>
+      <c r="E20" s="107" t="n">
+        <v>1232</v>
+      </c>
+      <c r="F20" s="99"/>
+      <c r="G20" s="99" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="105" t="n">
+        <v>43784</v>
+      </c>
+      <c r="B21" s="106" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" s="99" t="s">
+        <v>72</v>
+      </c>
+      <c r="D21" s="99"/>
+      <c r="E21" s="107" t="n">
+        <v>4720</v>
+      </c>
+      <c r="F21" s="99"/>
+      <c r="G21" s="99" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="105" t="n">
+        <v>43789</v>
+      </c>
+      <c r="B22" s="106" t="n">
+        <v>2</v>
+      </c>
+      <c r="C22" s="99" t="s">
+        <v>73</v>
+      </c>
+      <c r="D22" s="99"/>
+      <c r="E22" s="107" t="n">
+        <v>350</v>
+      </c>
+      <c r="F22" s="99"/>
+      <c r="G22" s="99" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="105" t="n">
+        <v>43789</v>
+      </c>
+      <c r="B23" s="106" t="n">
+        <v>18</v>
+      </c>
+      <c r="C23" s="99" t="s">
+        <v>74</v>
+      </c>
+      <c r="D23" s="99"/>
+      <c r="E23" s="107" t="n">
+        <v>7640</v>
+      </c>
+      <c r="F23" s="99"/>
+      <c r="G23" s="99" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="105" t="n">
+        <v>43791</v>
+      </c>
+      <c r="B24" s="106" t="n">
+        <v>12</v>
+      </c>
+      <c r="C24" s="99" t="s">
+        <v>75</v>
+      </c>
+      <c r="D24" s="99"/>
+      <c r="E24" s="107" t="n">
+        <v>846.48</v>
+      </c>
+      <c r="F24" s="99"/>
+      <c r="G24" s="99" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="105" t="n">
+        <v>43795</v>
+      </c>
+      <c r="B25" s="106" t="n">
+        <v>4</v>
+      </c>
+      <c r="C25" s="99" t="s">
+        <v>77</v>
+      </c>
+      <c r="D25" s="99"/>
+      <c r="E25" s="107" t="n">
+        <v>940</v>
+      </c>
+      <c r="F25" s="99"/>
+      <c r="G25" s="99" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="105" t="n">
         <v>43804</v>
       </c>
-      <c r="B18" s="105" t="n">
-        <v>1</v>
-      </c>
-      <c r="C18" s="98" t="s">
-        <v>67</v>
-      </c>
-      <c r="D18" s="98"/>
-      <c r="E18" s="106" t="n">
-        <v>580</v>
-      </c>
-      <c r="F18" s="98"/>
-      <c r="G18" s="98" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="104" t="n">
-        <v>43573</v>
-      </c>
-      <c r="B19" s="105" t="n">
-        <v>1</v>
-      </c>
-      <c r="C19" s="98" t="s">
-        <v>68</v>
-      </c>
-      <c r="D19" s="98"/>
-      <c r="E19" s="106" t="n">
-        <v>3305</v>
-      </c>
-      <c r="F19" s="98"/>
-      <c r="G19" s="98" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="104" t="n">
-        <v>43657</v>
-      </c>
-      <c r="B20" s="105" t="n">
+      <c r="B26" s="106" t="n">
         <v>2</v>
       </c>
-      <c r="C20" s="98" t="s">
-        <v>69</v>
-      </c>
-      <c r="D20" s="98"/>
-      <c r="E20" s="106" t="n">
-        <v>1232</v>
-      </c>
-      <c r="F20" s="98"/>
-      <c r="G20" s="98" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="104" t="n">
-        <v>43784</v>
-      </c>
-      <c r="B21" s="105" t="n">
-        <v>1</v>
-      </c>
-      <c r="C21" s="98" t="s">
-        <v>70</v>
-      </c>
-      <c r="D21" s="98"/>
-      <c r="E21" s="106" t="n">
-        <v>4720</v>
-      </c>
-      <c r="F21" s="98"/>
-      <c r="G21" s="98" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="104" t="n">
-        <v>43789</v>
-      </c>
-      <c r="B22" s="105" t="n">
+      <c r="C26" s="99" t="s">
+        <v>78</v>
+      </c>
+      <c r="D26" s="99"/>
+      <c r="E26" s="107" t="n">
+        <v>790</v>
+      </c>
+      <c r="F26" s="99"/>
+      <c r="G26" s="99" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="105" t="n">
+        <v>43804</v>
+      </c>
+      <c r="B27" s="106" t="n">
         <v>2</v>
       </c>
-      <c r="C22" s="98" t="s">
-        <v>71</v>
-      </c>
-      <c r="D22" s="98"/>
-      <c r="E22" s="106" t="n">
-        <v>350</v>
-      </c>
-      <c r="F22" s="98"/>
-      <c r="G22" s="98" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="104" t="n">
-        <v>43789</v>
-      </c>
-      <c r="B23" s="105" t="n">
-        <v>18</v>
-      </c>
-      <c r="C23" s="98" t="s">
-        <v>72</v>
-      </c>
-      <c r="D23" s="98"/>
-      <c r="E23" s="106" t="n">
-        <v>7640</v>
-      </c>
-      <c r="F23" s="98"/>
-      <c r="G23" s="98" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="104" t="n">
-        <v>43791</v>
-      </c>
-      <c r="B24" s="105" t="n">
-        <v>12</v>
-      </c>
-      <c r="C24" s="98" t="s">
-        <v>73</v>
-      </c>
-      <c r="D24" s="98"/>
-      <c r="E24" s="106" t="n">
-        <v>846.48</v>
-      </c>
-      <c r="F24" s="98"/>
-      <c r="G24" s="98" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="104" t="n">
-        <v>43795</v>
-      </c>
-      <c r="B25" s="105" t="n">
+      <c r="C27" s="99" t="s">
+        <v>80</v>
+      </c>
+      <c r="D27" s="99"/>
+      <c r="E27" s="107" t="n">
+        <v>210</v>
+      </c>
+      <c r="F27" s="99"/>
+      <c r="G27" s="99" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="105" t="n">
+        <v>43804</v>
+      </c>
+      <c r="B28" s="106" t="n">
         <v>4</v>
       </c>
-      <c r="C25" s="98" t="s">
-        <v>75</v>
-      </c>
-      <c r="D25" s="98"/>
-      <c r="E25" s="106" t="n">
-        <v>940</v>
-      </c>
-      <c r="F25" s="98"/>
-      <c r="G25" s="98" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="104" t="n">
-        <v>43804</v>
-      </c>
-      <c r="B26" s="105" t="n">
-        <v>2</v>
-      </c>
-      <c r="C26" s="98" t="s">
-        <v>76</v>
-      </c>
-      <c r="D26" s="98"/>
-      <c r="E26" s="106" t="n">
-        <v>790</v>
-      </c>
-      <c r="F26" s="98"/>
-      <c r="G26" s="98" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="104" t="n">
-        <v>43804</v>
-      </c>
-      <c r="B27" s="105" t="n">
-        <v>2</v>
-      </c>
-      <c r="C27" s="98" t="s">
-        <v>78</v>
-      </c>
-      <c r="D27" s="98"/>
-      <c r="E27" s="106" t="n">
-        <v>210</v>
-      </c>
-      <c r="F27" s="98"/>
-      <c r="G27" s="98" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="104" t="n">
-        <v>43804</v>
-      </c>
-      <c r="B28" s="105" t="n">
-        <v>4</v>
-      </c>
-      <c r="C28" s="98" t="s">
-        <v>79</v>
-      </c>
-      <c r="D28" s="98"/>
-      <c r="E28" s="106" t="n">
+      <c r="C28" s="99" t="s">
+        <v>81</v>
+      </c>
+      <c r="D28" s="99"/>
+      <c r="E28" s="107" t="n">
         <v>1160</v>
       </c>
-      <c r="F28" s="98"/>
-      <c r="G28" s="98" t="s">
-        <v>55</v>
+      <c r="F28" s="99"/>
+      <c r="G28" s="99" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="108"/>
-      <c r="B29" s="98"/>
-      <c r="C29" s="98"/>
-      <c r="D29" s="98"/>
-      <c r="E29" s="109" t="n">
+      <c r="A29" s="109"/>
+      <c r="B29" s="99"/>
+      <c r="C29" s="99"/>
+      <c r="D29" s="99"/>
+      <c r="E29" s="110" t="n">
         <v>47426.48</v>
       </c>
-      <c r="F29" s="98" t="s">
-        <v>80</v>
-      </c>
-      <c r="G29" s="110" t="s">
-        <v>80</v>
+      <c r="F29" s="99" t="s">
+        <v>82</v>
+      </c>
+      <c r="G29" s="111" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="108"/>
-      <c r="B30" s="98"/>
-      <c r="C30" s="98"/>
-      <c r="D30" s="98"/>
-      <c r="E30" s="106"/>
-      <c r="F30" s="98"/>
-      <c r="G30" s="98"/>
+      <c r="A30" s="109"/>
+      <c r="B30" s="99"/>
+      <c r="C30" s="99"/>
+      <c r="D30" s="99"/>
+      <c r="E30" s="107"/>
+      <c r="F30" s="99"/>
+      <c r="G30" s="99"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="108"/>
-      <c r="B31" s="98"/>
-      <c r="C31" s="98"/>
-      <c r="D31" s="98"/>
-      <c r="E31" s="98"/>
-      <c r="F31" s="98"/>
-      <c r="G31" s="98"/>
+      <c r="A31" s="109"/>
+      <c r="B31" s="99"/>
+      <c r="C31" s="99"/>
+      <c r="D31" s="99"/>
+      <c r="E31" s="99"/>
+      <c r="F31" s="99"/>
+      <c r="G31" s="99"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="108"/>
-      <c r="B32" s="98"/>
-      <c r="C32" s="98"/>
-      <c r="D32" s="98"/>
-      <c r="E32" s="98"/>
-      <c r="F32" s="98"/>
-      <c r="G32" s="98"/>
+      <c r="A32" s="109"/>
+      <c r="B32" s="99"/>
+      <c r="C32" s="99"/>
+      <c r="D32" s="99"/>
+      <c r="E32" s="99"/>
+      <c r="F32" s="99"/>
+      <c r="G32" s="99"/>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="108"/>
+      <c r="A33" s="109"/>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="108"/>
+      <c r="A34" s="109"/>
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="108"/>
+      <c r="A35" s="109"/>
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="108"/>
+      <c r="A36" s="109"/>
     </row>
     <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="108"/>
+      <c r="A37" s="109"/>
     </row>
     <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="108"/>
+      <c r="A38" s="109"/>
     </row>
     <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="108"/>
+      <c r="A39" s="109"/>
     </row>
     <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="108"/>
+      <c r="A40" s="109"/>
     </row>
     <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="108"/>
+      <c r="A41" s="109"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2683,567 +2705,567 @@
   </sheetPr>
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J14" activeCellId="1" sqref="D15:G15 J14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D29" activeCellId="0" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.59375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.56640625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.87"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="97" t="s">
-        <v>45</v>
-      </c>
-      <c r="B1" s="98"/>
-      <c r="C1" s="98"/>
-      <c r="D1" s="98"/>
-      <c r="E1" s="98"/>
-      <c r="F1" s="98"/>
-      <c r="G1" s="98"/>
+      <c r="A1" s="98" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="99"/>
+      <c r="C1" s="99"/>
+      <c r="D1" s="99"/>
+      <c r="E1" s="99"/>
+      <c r="F1" s="99"/>
+      <c r="G1" s="99"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="97" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2" s="98"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
+      <c r="A2" s="98" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="99"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="97" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" s="98"/>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
+      <c r="A3" s="98" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="99"/>
+      <c r="C3" s="99"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="99"/>
+      <c r="G3" s="99"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="97" t="s">
-        <v>48</v>
-      </c>
-      <c r="B4" s="98"/>
-      <c r="C4" s="98"/>
-      <c r="D4" s="98"/>
-      <c r="E4" s="98"/>
-      <c r="F4" s="98"/>
-      <c r="G4" s="98"/>
+      <c r="A4" s="98" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="99"/>
+      <c r="C4" s="99"/>
+      <c r="D4" s="99"/>
+      <c r="E4" s="99"/>
+      <c r="F4" s="99"/>
+      <c r="G4" s="99"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="111" t="s">
-        <v>49</v>
-      </c>
-      <c r="B6" s="111" t="s">
-        <v>81</v>
-      </c>
-      <c r="C6" s="111" t="s">
+      <c r="A6" s="112" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="112" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" s="112" t="s">
+        <v>84</v>
+      </c>
+      <c r="D6" s="112" t="s">
+        <v>85</v>
+      </c>
+      <c r="E6" s="112" t="s">
+        <v>86</v>
+      </c>
+      <c r="F6" s="101"/>
+      <c r="G6" s="101"/>
+    </row>
+    <row r="7" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="113" t="n">
+        <v>43938</v>
+      </c>
+      <c r="B7" s="114" t="n">
+        <v>849</v>
+      </c>
+      <c r="C7" s="106" t="s">
+        <v>87</v>
+      </c>
+      <c r="D7" s="115" t="s">
+        <v>88</v>
+      </c>
+      <c r="E7" s="116" t="n">
+        <v>1344</v>
+      </c>
+      <c r="F7" s="111"/>
+      <c r="G7" s="99"/>
+    </row>
+    <row r="8" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="113" t="n">
+        <v>43939</v>
+      </c>
+      <c r="B8" s="114" t="n">
+        <v>854</v>
+      </c>
+      <c r="C8" s="106" t="s">
+        <v>87</v>
+      </c>
+      <c r="D8" s="115" t="s">
+        <v>88</v>
+      </c>
+      <c r="E8" s="116" t="n">
+        <v>3305</v>
+      </c>
+      <c r="F8" s="111"/>
+      <c r="G8" s="99"/>
+    </row>
+    <row r="9" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="113" t="n">
+        <v>43979</v>
+      </c>
+      <c r="B9" s="114" t="n">
+        <v>870</v>
+      </c>
+      <c r="C9" s="106" t="s">
+        <v>87</v>
+      </c>
+      <c r="D9" s="115" t="s">
+        <v>88</v>
+      </c>
+      <c r="E9" s="116" t="n">
+        <v>945</v>
+      </c>
+      <c r="F9" s="111"/>
+      <c r="G9" s="99"/>
+    </row>
+    <row r="10" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="113" t="n">
+        <v>44100</v>
+      </c>
+      <c r="B10" s="114" t="n">
+        <v>969</v>
+      </c>
+      <c r="C10" s="106" t="s">
+        <v>87</v>
+      </c>
+      <c r="D10" s="115" t="s">
+        <v>88</v>
+      </c>
+      <c r="E10" s="116" t="n">
+        <v>1010</v>
+      </c>
+      <c r="F10" s="111"/>
+      <c r="G10" s="99"/>
+    </row>
+    <row r="11" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="113" t="n">
+        <v>44036</v>
+      </c>
+      <c r="B11" s="114" t="n">
+        <v>929</v>
+      </c>
+      <c r="C11" s="106" t="s">
+        <v>87</v>
+      </c>
+      <c r="D11" s="115" t="s">
+        <v>88</v>
+      </c>
+      <c r="E11" s="116" t="n">
+        <v>3905</v>
+      </c>
+      <c r="F11" s="111"/>
+      <c r="G11" s="99"/>
+    </row>
+    <row r="12" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="113" t="n">
+        <v>44036</v>
+      </c>
+      <c r="B12" s="114" t="n">
+        <v>926</v>
+      </c>
+      <c r="C12" s="106" t="s">
+        <v>87</v>
+      </c>
+      <c r="D12" s="115" t="s">
+        <v>88</v>
+      </c>
+      <c r="E12" s="116" t="n">
+        <v>2055</v>
+      </c>
+      <c r="F12" s="111"/>
+      <c r="G12" s="99"/>
+    </row>
+    <row r="13" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="113" t="n">
+        <v>44017</v>
+      </c>
+      <c r="B13" s="114" t="n">
+        <v>914</v>
+      </c>
+      <c r="C13" s="106" t="s">
+        <v>87</v>
+      </c>
+      <c r="D13" s="115" t="s">
+        <v>88</v>
+      </c>
+      <c r="E13" s="116" t="n">
+        <v>4700</v>
+      </c>
+      <c r="F13" s="111"/>
+      <c r="G13" s="99"/>
+    </row>
+    <row r="14" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="113" t="n">
+        <v>44108</v>
+      </c>
+      <c r="B14" s="114" t="n">
+        <v>154</v>
+      </c>
+      <c r="C14" s="106" t="s">
+        <v>89</v>
+      </c>
+      <c r="D14" s="115" t="s">
+        <v>90</v>
+      </c>
+      <c r="E14" s="116" t="n">
+        <v>660</v>
+      </c>
+      <c r="F14" s="111"/>
+      <c r="G14" s="99"/>
+    </row>
+    <row r="15" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="113" t="n">
+        <v>44170</v>
+      </c>
+      <c r="B15" s="114" t="n">
+        <v>191</v>
+      </c>
+      <c r="C15" s="106" t="s">
+        <v>89</v>
+      </c>
+      <c r="D15" s="115" t="s">
+        <v>90</v>
+      </c>
+      <c r="E15" s="116" t="n">
+        <v>2740</v>
+      </c>
+      <c r="F15" s="111"/>
+      <c r="G15" s="99"/>
+    </row>
+    <row r="16" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="113" t="n">
+        <v>44118</v>
+      </c>
+      <c r="B16" s="114" t="n">
+        <v>550</v>
+      </c>
+      <c r="C16" s="106" t="s">
+        <v>91</v>
+      </c>
+      <c r="D16" s="115" t="s">
+        <v>92</v>
+      </c>
+      <c r="E16" s="116" t="n">
+        <v>2441</v>
+      </c>
+      <c r="F16" s="111"/>
+      <c r="G16" s="99"/>
+    </row>
+    <row r="17" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="113" t="n">
+        <v>44118</v>
+      </c>
+      <c r="B17" s="114" t="n">
+        <v>551</v>
+      </c>
+      <c r="C17" s="106" t="s">
+        <v>91</v>
+      </c>
+      <c r="D17" s="115" t="s">
+        <v>92</v>
+      </c>
+      <c r="E17" s="116" t="n">
+        <v>3069</v>
+      </c>
+      <c r="F17" s="111"/>
+      <c r="G17" s="99"/>
+      <c r="H17" s="99"/>
+      <c r="I17" s="99"/>
+    </row>
+    <row r="18" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="113" t="n">
+        <v>44155</v>
+      </c>
+      <c r="B18" s="114" t="n">
+        <v>558</v>
+      </c>
+      <c r="C18" s="106" t="s">
+        <v>91</v>
+      </c>
+      <c r="D18" s="115" t="s">
+        <v>92</v>
+      </c>
+      <c r="E18" s="116" t="n">
+        <v>7640</v>
+      </c>
+      <c r="F18" s="111"/>
+      <c r="G18" s="99"/>
+      <c r="H18" s="99"/>
+      <c r="I18" s="99"/>
+    </row>
+    <row r="19" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="113" t="n">
+        <v>44150</v>
+      </c>
+      <c r="B19" s="114" t="n">
+        <v>557</v>
+      </c>
+      <c r="C19" s="106" t="s">
+        <v>91</v>
+      </c>
+      <c r="D19" s="115" t="s">
+        <v>92</v>
+      </c>
+      <c r="E19" s="116" t="n">
+        <v>4720</v>
+      </c>
+      <c r="F19" s="111"/>
+      <c r="G19" s="99"/>
+      <c r="H19" s="99"/>
+      <c r="I19" s="99"/>
+    </row>
+    <row r="20" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="113" t="n">
+        <v>44092</v>
+      </c>
+      <c r="B20" s="114" t="n">
+        <v>548</v>
+      </c>
+      <c r="C20" s="106" t="s">
+        <v>91</v>
+      </c>
+      <c r="D20" s="115" t="s">
+        <v>92</v>
+      </c>
+      <c r="E20" s="116" t="n">
+        <v>5524</v>
+      </c>
+      <c r="F20" s="111"/>
+      <c r="G20" s="99"/>
+      <c r="H20" s="99"/>
+      <c r="I20" s="99"/>
+    </row>
+    <row r="21" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="113" t="n">
+        <v>44161</v>
+      </c>
+      <c r="B21" s="114" t="n">
+        <v>8274</v>
+      </c>
+      <c r="C21" s="106" t="s">
+        <v>93</v>
+      </c>
+      <c r="D21" s="115" t="s">
+        <v>94</v>
+      </c>
+      <c r="E21" s="116" t="n">
+        <v>940</v>
+      </c>
+      <c r="F21" s="111"/>
+      <c r="G21" s="99"/>
+      <c r="H21" s="99"/>
+      <c r="I21" s="99"/>
+    </row>
+    <row r="22" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="113" t="n">
+        <v>44155</v>
+      </c>
+      <c r="B22" s="114" t="n">
+        <v>8267</v>
+      </c>
+      <c r="C22" s="106" t="s">
+        <v>93</v>
+      </c>
+      <c r="D22" s="115" t="s">
+        <v>94</v>
+      </c>
+      <c r="E22" s="116" t="n">
+        <v>350</v>
+      </c>
+      <c r="F22" s="111"/>
+      <c r="G22" s="99"/>
+      <c r="H22" s="99"/>
+      <c r="I22" s="99"/>
+    </row>
+    <row r="23" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="113" t="n">
+        <v>44157</v>
+      </c>
+      <c r="B23" s="114" t="n">
+        <v>1504</v>
+      </c>
+      <c r="C23" s="106" t="s">
+        <v>95</v>
+      </c>
+      <c r="D23" s="115" t="s">
+        <v>96</v>
+      </c>
+      <c r="E23" s="116" t="n">
+        <v>846.48</v>
+      </c>
+      <c r="F23" s="111"/>
+      <c r="G23" s="99"/>
+      <c r="H23" s="99"/>
+      <c r="I23" s="99"/>
+    </row>
+    <row r="24" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="117" t="n">
+        <v>44023</v>
+      </c>
+      <c r="B24" s="114" t="n">
+        <v>5565</v>
+      </c>
+      <c r="C24" s="106" t="s">
+        <v>97</v>
+      </c>
+      <c r="D24" s="115" t="s">
+        <v>98</v>
+      </c>
+      <c r="E24" s="116" t="n">
+        <v>1232</v>
+      </c>
+      <c r="F24" s="111"/>
+      <c r="G24" s="99"/>
+      <c r="H24" s="99"/>
+      <c r="I24" s="99"/>
+    </row>
+    <row r="25" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="99"/>
+      <c r="B25" s="99"/>
+      <c r="C25" s="114" t="s">
+        <v>99</v>
+      </c>
+      <c r="D25" s="114"/>
+      <c r="E25" s="118" t="n">
+        <v>47426.48</v>
+      </c>
+      <c r="F25" s="111" t="s">
         <v>82</v>
       </c>
-      <c r="D6" s="111" t="s">
-        <v>83</v>
-      </c>
-      <c r="E6" s="111" t="s">
-        <v>84</v>
-      </c>
-      <c r="F6" s="100"/>
-      <c r="G6" s="100"/>
-    </row>
-    <row r="7" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="112" t="n">
-        <v>43938</v>
-      </c>
-      <c r="B7" s="113" t="n">
-        <v>849</v>
-      </c>
-      <c r="C7" s="105" t="s">
-        <v>85</v>
-      </c>
-      <c r="D7" s="114" t="s">
-        <v>86</v>
-      </c>
-      <c r="E7" s="115" t="n">
-        <v>1344</v>
-      </c>
-      <c r="F7" s="110"/>
-      <c r="G7" s="98"/>
-    </row>
-    <row r="8" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="112" t="n">
-        <v>43939</v>
-      </c>
-      <c r="B8" s="113" t="n">
-        <v>854</v>
-      </c>
-      <c r="C8" s="105" t="s">
-        <v>85</v>
-      </c>
-      <c r="D8" s="114" t="s">
-        <v>86</v>
-      </c>
-      <c r="E8" s="115" t="n">
-        <v>3305</v>
-      </c>
-      <c r="F8" s="110"/>
-      <c r="G8" s="98"/>
-    </row>
-    <row r="9" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="112" t="n">
-        <v>43979</v>
-      </c>
-      <c r="B9" s="113" t="n">
-        <v>870</v>
-      </c>
-      <c r="C9" s="105" t="s">
-        <v>85</v>
-      </c>
-      <c r="D9" s="114" t="s">
-        <v>86</v>
-      </c>
-      <c r="E9" s="115" t="n">
-        <v>945</v>
-      </c>
-      <c r="F9" s="110"/>
-      <c r="G9" s="98"/>
-    </row>
-    <row r="10" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="112" t="n">
-        <v>44100</v>
-      </c>
-      <c r="B10" s="113" t="n">
-        <v>969</v>
-      </c>
-      <c r="C10" s="105" t="s">
-        <v>85</v>
-      </c>
-      <c r="D10" s="114" t="s">
-        <v>86</v>
-      </c>
-      <c r="E10" s="115" t="n">
-        <v>1010</v>
-      </c>
-      <c r="F10" s="110"/>
-      <c r="G10" s="98"/>
-    </row>
-    <row r="11" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="112" t="n">
-        <v>44036</v>
-      </c>
-      <c r="B11" s="113" t="n">
-        <v>929</v>
-      </c>
-      <c r="C11" s="105" t="s">
-        <v>85</v>
-      </c>
-      <c r="D11" s="114" t="s">
-        <v>86</v>
-      </c>
-      <c r="E11" s="115" t="n">
-        <v>3905</v>
-      </c>
-      <c r="F11" s="110"/>
-      <c r="G11" s="98"/>
-    </row>
-    <row r="12" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="112" t="n">
-        <v>44036</v>
-      </c>
-      <c r="B12" s="113" t="n">
-        <v>926</v>
-      </c>
-      <c r="C12" s="105" t="s">
-        <v>85</v>
-      </c>
-      <c r="D12" s="114" t="s">
-        <v>86</v>
-      </c>
-      <c r="E12" s="115" t="n">
-        <v>2055</v>
-      </c>
-      <c r="F12" s="110"/>
-      <c r="G12" s="98"/>
-    </row>
-    <row r="13" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="112" t="n">
-        <v>44017</v>
-      </c>
-      <c r="B13" s="113" t="n">
-        <v>914</v>
-      </c>
-      <c r="C13" s="105" t="s">
-        <v>85</v>
-      </c>
-      <c r="D13" s="114" t="s">
-        <v>86</v>
-      </c>
-      <c r="E13" s="115" t="n">
-        <v>4700</v>
-      </c>
-      <c r="F13" s="110"/>
-      <c r="G13" s="98"/>
-    </row>
-    <row r="14" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="112" t="n">
-        <v>44108</v>
-      </c>
-      <c r="B14" s="113" t="n">
-        <v>154</v>
-      </c>
-      <c r="C14" s="105" t="s">
-        <v>87</v>
-      </c>
-      <c r="D14" s="114" t="s">
-        <v>88</v>
-      </c>
-      <c r="E14" s="115" t="n">
-        <v>660</v>
-      </c>
-      <c r="F14" s="110"/>
-      <c r="G14" s="98"/>
-    </row>
-    <row r="15" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="112" t="n">
-        <v>44170</v>
-      </c>
-      <c r="B15" s="113" t="n">
-        <v>191</v>
-      </c>
-      <c r="C15" s="105" t="s">
-        <v>87</v>
-      </c>
-      <c r="D15" s="114" t="s">
-        <v>88</v>
-      </c>
-      <c r="E15" s="115" t="n">
-        <v>2740</v>
-      </c>
-      <c r="F15" s="110"/>
-      <c r="G15" s="98"/>
-    </row>
-    <row r="16" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="112" t="n">
-        <v>44118</v>
-      </c>
-      <c r="B16" s="113" t="n">
-        <v>550</v>
-      </c>
-      <c r="C16" s="105" t="s">
-        <v>89</v>
-      </c>
-      <c r="D16" s="114" t="s">
-        <v>90</v>
-      </c>
-      <c r="E16" s="115" t="n">
-        <v>2441</v>
-      </c>
-      <c r="F16" s="110"/>
-      <c r="G16" s="98"/>
-    </row>
-    <row r="17" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="112" t="n">
-        <v>44118</v>
-      </c>
-      <c r="B17" s="113" t="n">
-        <v>551</v>
-      </c>
-      <c r="C17" s="105" t="s">
-        <v>89</v>
-      </c>
-      <c r="D17" s="114" t="s">
-        <v>90</v>
-      </c>
-      <c r="E17" s="115" t="n">
-        <v>3069</v>
-      </c>
-      <c r="F17" s="110"/>
-      <c r="G17" s="98"/>
-      <c r="H17" s="98"/>
-      <c r="I17" s="98"/>
-    </row>
-    <row r="18" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="112" t="n">
-        <v>44155</v>
-      </c>
-      <c r="B18" s="113" t="n">
-        <v>558</v>
-      </c>
-      <c r="C18" s="105" t="s">
-        <v>89</v>
-      </c>
-      <c r="D18" s="114" t="s">
-        <v>90</v>
-      </c>
-      <c r="E18" s="115" t="n">
-        <v>7640</v>
-      </c>
-      <c r="F18" s="110"/>
-      <c r="G18" s="98"/>
-      <c r="H18" s="98"/>
-      <c r="I18" s="98"/>
-    </row>
-    <row r="19" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="112" t="n">
-        <v>44150</v>
-      </c>
-      <c r="B19" s="113" t="n">
-        <v>557</v>
-      </c>
-      <c r="C19" s="105" t="s">
-        <v>89</v>
-      </c>
-      <c r="D19" s="114" t="s">
-        <v>90</v>
-      </c>
-      <c r="E19" s="115" t="n">
-        <v>4720</v>
-      </c>
-      <c r="F19" s="110"/>
-      <c r="G19" s="98"/>
-      <c r="H19" s="98"/>
-      <c r="I19" s="98"/>
-    </row>
-    <row r="20" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="112" t="n">
-        <v>44092</v>
-      </c>
-      <c r="B20" s="113" t="n">
-        <v>548</v>
-      </c>
-      <c r="C20" s="105" t="s">
-        <v>89</v>
-      </c>
-      <c r="D20" s="114" t="s">
-        <v>90</v>
-      </c>
-      <c r="E20" s="115" t="n">
-        <v>5524</v>
-      </c>
-      <c r="F20" s="110"/>
-      <c r="G20" s="98"/>
-      <c r="H20" s="98"/>
-      <c r="I20" s="98"/>
-    </row>
-    <row r="21" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="112" t="n">
-        <v>44161</v>
-      </c>
-      <c r="B21" s="113" t="n">
-        <v>8274</v>
-      </c>
-      <c r="C21" s="105" t="s">
-        <v>91</v>
-      </c>
-      <c r="D21" s="114" t="s">
-        <v>92</v>
-      </c>
-      <c r="E21" s="115" t="n">
-        <v>940</v>
-      </c>
-      <c r="F21" s="110"/>
-      <c r="G21" s="98"/>
-      <c r="H21" s="98"/>
-      <c r="I21" s="98"/>
-    </row>
-    <row r="22" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="112" t="n">
-        <v>44155</v>
-      </c>
-      <c r="B22" s="113" t="n">
-        <v>8267</v>
-      </c>
-      <c r="C22" s="105" t="s">
-        <v>91</v>
-      </c>
-      <c r="D22" s="114" t="s">
-        <v>92</v>
-      </c>
-      <c r="E22" s="115" t="n">
-        <v>350</v>
-      </c>
-      <c r="F22" s="110"/>
-      <c r="G22" s="98"/>
-      <c r="H22" s="98"/>
-      <c r="I22" s="98"/>
-    </row>
-    <row r="23" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="112" t="n">
-        <v>44157</v>
-      </c>
-      <c r="B23" s="113" t="n">
-        <v>1504</v>
-      </c>
-      <c r="C23" s="105" t="s">
-        <v>93</v>
-      </c>
-      <c r="D23" s="114" t="s">
-        <v>94</v>
-      </c>
-      <c r="E23" s="115" t="n">
-        <v>846.48</v>
-      </c>
-      <c r="F23" s="110"/>
-      <c r="G23" s="98"/>
-      <c r="H23" s="98"/>
-      <c r="I23" s="98"/>
-    </row>
-    <row r="24" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="116" t="n">
-        <v>44023</v>
-      </c>
-      <c r="B24" s="113" t="n">
-        <v>5565</v>
-      </c>
-      <c r="C24" s="105" t="s">
-        <v>95</v>
-      </c>
-      <c r="D24" s="114" t="s">
-        <v>96</v>
-      </c>
-      <c r="E24" s="115" t="n">
-        <v>1232</v>
-      </c>
-      <c r="F24" s="110"/>
-      <c r="G24" s="98"/>
-      <c r="H24" s="98"/>
-      <c r="I24" s="98"/>
-    </row>
-    <row r="25" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="98"/>
-      <c r="B25" s="98"/>
-      <c r="C25" s="113" t="s">
-        <v>97</v>
-      </c>
-      <c r="D25" s="113"/>
-      <c r="E25" s="117" t="n">
-        <v>47426.48</v>
-      </c>
-      <c r="F25" s="110" t="s">
-        <v>80</v>
-      </c>
-      <c r="G25" s="110" t="s">
-        <v>80</v>
-      </c>
-      <c r="H25" s="110" t="s">
-        <v>80</v>
-      </c>
-      <c r="I25" s="98"/>
+      <c r="G25" s="111" t="s">
+        <v>82</v>
+      </c>
+      <c r="H25" s="111" t="s">
+        <v>82</v>
+      </c>
+      <c r="I25" s="99"/>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="98"/>
-      <c r="B26" s="98"/>
-      <c r="C26" s="98"/>
-      <c r="D26" s="98"/>
-      <c r="E26" s="110"/>
-      <c r="F26" s="100"/>
-      <c r="G26" s="100"/>
-      <c r="H26" s="98"/>
-      <c r="I26" s="98"/>
+      <c r="A26" s="99"/>
+      <c r="B26" s="99"/>
+      <c r="C26" s="99"/>
+      <c r="D26" s="99"/>
+      <c r="E26" s="111"/>
+      <c r="F26" s="101"/>
+      <c r="G26" s="101"/>
+      <c r="H26" s="99"/>
+      <c r="I26" s="99"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="98"/>
-      <c r="B27" s="98"/>
-      <c r="C27" s="98"/>
-      <c r="D27" s="98"/>
-      <c r="E27" s="98"/>
-      <c r="F27" s="98"/>
-      <c r="G27" s="98"/>
-      <c r="H27" s="98"/>
-      <c r="I27" s="98"/>
+      <c r="A27" s="99"/>
+      <c r="B27" s="99"/>
+      <c r="C27" s="99"/>
+      <c r="D27" s="99"/>
+      <c r="E27" s="99"/>
+      <c r="F27" s="99"/>
+      <c r="G27" s="99"/>
+      <c r="H27" s="99"/>
+      <c r="I27" s="99"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="98"/>
-      <c r="B28" s="98"/>
-      <c r="C28" s="98"/>
-      <c r="D28" s="98"/>
-      <c r="E28" s="98"/>
-      <c r="F28" s="98"/>
-      <c r="G28" s="98"/>
-      <c r="H28" s="98"/>
-      <c r="I28" s="98"/>
+      <c r="A28" s="99"/>
+      <c r="B28" s="99"/>
+      <c r="C28" s="99"/>
+      <c r="D28" s="99"/>
+      <c r="E28" s="99"/>
+      <c r="F28" s="99"/>
+      <c r="G28" s="99"/>
+      <c r="H28" s="99"/>
+      <c r="I28" s="99"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="98"/>
-      <c r="B29" s="98"/>
-      <c r="C29" s="98"/>
-      <c r="D29" s="98"/>
-      <c r="E29" s="98"/>
-      <c r="F29" s="98"/>
-      <c r="G29" s="98"/>
-      <c r="H29" s="98"/>
-      <c r="I29" s="98"/>
+      <c r="A29" s="99"/>
+      <c r="B29" s="99"/>
+      <c r="C29" s="99"/>
+      <c r="D29" s="99"/>
+      <c r="E29" s="99"/>
+      <c r="F29" s="99"/>
+      <c r="G29" s="99"/>
+      <c r="H29" s="99"/>
+      <c r="I29" s="99"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="98"/>
-      <c r="B30" s="98"/>
-      <c r="C30" s="98"/>
-      <c r="D30" s="98"/>
-      <c r="E30" s="98"/>
-      <c r="F30" s="98"/>
-      <c r="G30" s="98"/>
-      <c r="H30" s="98"/>
-      <c r="I30" s="98"/>
+      <c r="A30" s="99"/>
+      <c r="B30" s="99"/>
+      <c r="C30" s="99"/>
+      <c r="D30" s="99"/>
+      <c r="E30" s="99"/>
+      <c r="F30" s="99"/>
+      <c r="G30" s="99"/>
+      <c r="H30" s="99"/>
+      <c r="I30" s="99"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="98"/>
-      <c r="B31" s="98"/>
-      <c r="C31" s="98"/>
-      <c r="D31" s="98"/>
-      <c r="E31" s="98" t="s">
-        <v>80</v>
-      </c>
-      <c r="F31" s="98"/>
-      <c r="G31" s="98"/>
-      <c r="H31" s="98"/>
-      <c r="I31" s="110" t="s">
-        <v>80</v>
+      <c r="A31" s="99"/>
+      <c r="B31" s="99"/>
+      <c r="C31" s="99"/>
+      <c r="D31" s="99"/>
+      <c r="E31" s="99" t="s">
+        <v>82</v>
+      </c>
+      <c r="F31" s="99"/>
+      <c r="G31" s="99"/>
+      <c r="H31" s="99"/>
+      <c r="I31" s="111" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="98"/>
-      <c r="B32" s="98"/>
-      <c r="C32" s="98"/>
-      <c r="D32" s="98"/>
-      <c r="E32" s="98"/>
-      <c r="F32" s="98"/>
-      <c r="G32" s="98"/>
-      <c r="H32" s="98"/>
-      <c r="I32" s="98"/>
+      <c r="A32" s="99"/>
+      <c r="B32" s="99"/>
+      <c r="C32" s="99"/>
+      <c r="D32" s="99"/>
+      <c r="E32" s="99"/>
+      <c r="F32" s="99"/>
+      <c r="G32" s="99"/>
+      <c r="H32" s="99"/>
+      <c r="I32" s="99"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E33" s="98"/>
+      <c r="E33" s="99"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E34" s="110" t="s">
-        <v>80</v>
+      <c r="E34" s="111" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E35" s="110"/>
+      <c r="E35" s="111"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E36" s="110"/>
+      <c r="E36" s="111"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E37" s="110"/>
+      <c r="E37" s="111"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E38" s="110"/>
+      <c r="E38" s="111"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E39" s="110"/>
+      <c r="E39" s="111"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E40" s="110"/>
+      <c r="E40" s="111"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E41" s="110"/>
+      <c r="E41" s="111"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>